<commit_message>
Schema changed. Implemented printed documents for commission journal and print methods for other documents
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/ReportTemplates.xlsx
+++ b/DatabaseUpdate/ExcelFiles/ReportTemplates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -34,9 +34,6 @@
     <x:t>Template</x:t>
   </x:si>
   <x:si>
-    <x:t>IsAgreementDocument</x:t>
-  </x:si>
-  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
@@ -50,13 +47,10 @@
   </x:si>
   <x:si>
     <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
-&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblpPr w:leftFromText="180" w:rightFromText="180" w:vertAnchor="text" w:horzAnchor="margin" w:tblpY="-142"/&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="4361"/&gt;&lt;w:gridCol w:w="1417"/&gt;&lt;w:gridCol w:w="3793"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4361" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00C675B3" w:rsidRPr="00626937" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Наименование медицинской организации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1417" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3793" w:type="dxa"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Код формы по ОКУД __________                                        Код организации по ОКПО: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgOKPO&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Медицинская документация                                               Учетная форма N &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;025/у&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Утверждена&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; приказом Минздрава России                                  от 15 декабря 2014 г. N 834н&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;       &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="Par64"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                         &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;МЕДИЦИНСКАЯ КАРТА&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПАЦИЕНТА, ПОЛУЧАЮЩЕГО МЕДИЦИНСКУЮ ПОМОЩЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;В АМБУЛАТОРНЫХ УСЛОВИЯХ N &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CardNumber&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="1" w:name="Par68"/&gt;&lt;w:bookmarkEnd w:id="1"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1. Дата заполнения медицинской карты: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CardDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="2" w:name="Par69"/&gt;&lt;w:bookmarkEnd w:id="2"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2. Фамилия, имя, отчество: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFIO&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3. Пол: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Gender&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;4. Дата рождения: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BirthDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;5. Место регистрации: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Address&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;; тел.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContactPhone&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="3" w:name="Par74"/&gt;&lt;w:bookmarkEnd w:id="3"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;6. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Местность&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;: Registration&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00A77D4D" w:rsidRPr="00557D8F" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="4" w:name="Par75"/&gt;&lt;w:bookmarkEnd w:id="4"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;InsuranceDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00557D8F" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;8. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;СНИЛС&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="5" w:name="Par76"/&gt;&lt;w:bookmarkEnd w:id="5"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;SNILS&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9. Наи&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;менование страховой медицинской организации: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;InsuranceCompany&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="6" w:name="Par77"/&gt;&lt;w:bookmarkEnd w:id="6"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;10. Код категории льготы: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BenefitCode&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11. Документ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="7" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="7"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;льготы&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BenefitDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="8" w:name="Par78"/&gt;&lt;w:bookmarkStart w:id="9" w:name="Par111"/&gt;&lt;w:bookmarkStart w:id="10" w:name="Par113"/&gt;&lt;w:bookmarkEnd w:id="8"/&gt;&lt;w:bookmarkEnd w:id="9"/&gt;&lt;w:bookmarkEnd w:id="10"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;12. Семейное положение: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;MaritalStatus&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="11" w:name="Par115"/&gt;&lt;w:bookmarkEnd w:id="11"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;13. Образование: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Education&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="12" w:name="Par117"/&gt;&lt;w:bookmarkEnd w:id="12"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;14. Занятость: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Employment&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;15. Место работы, должность: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Business&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="13" w:name="Par120"/&gt;&lt;w:bookmarkEnd w:id="13"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;16. Инвалидность: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Disability&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="14" w:name="Par121"/&gt;&lt;w:bookmarkEnd w:id="14"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;17. Группа крови: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BloodGroup&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;18.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Rh&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;-фактор: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BloodRh&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;19. Аллергические реакции: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Allergy&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="15" w:name="Par122"/&gt;&lt;w:bookmarkEnd w:id="15"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;20. Изменение места работы ________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="16" w:name="Par123"/&gt;&lt;w:bookmarkEnd w:id="16"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;21. Изменение места регистрации _____________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="17" w:name="Par124"/&gt;&lt;w:bookmarkStart w:id="18" w:name="Par151"/&gt;&lt;w:bookmarkEnd w:id="17"/&gt;&lt;w:bookmarkEnd w:id="18"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:sectPr w:rsidR="001F2DC7" w:rsidRPr="00C675B3"&gt;&lt;w:pgSz w:w="11907" w:h="8391" w:orient="landscape"/&gt;&lt;w:pgMar w:top="567" w:right="851" w:bottom="284" w:left="851" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="720"/&gt;&lt;/w:sectPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="19" w:name="Par154"/&gt;&lt;w:bookmarkStart w:id="20" w:name="Par156"/&gt;&lt;w:bookmarkStart w:id="21" w:name="Par328"/&gt;&lt;w:bookmarkStart w:id="22" w:name="Par330"/&gt;&lt;w:bookmarkStart w:id="23" w:name="Par360"/&gt;&lt;w:bookmarkStart w:id="24" w:name="Par392"/&gt;&lt;w:bookmarkStart w:id="25" w:name="Par427"/&gt;&lt;w:bookmarkStart w:id="26" w:name="Par459"/&gt;&lt;w:bookmarkStart w:id="27" w:name="Par461"/&gt;&lt;w:bookmarkEnd w:id="19"/&gt;&lt;w:bookmarkEnd w:id="20"/&gt;&lt;w:bookmarkEnd w:id="21"/&gt;&lt;w:bookmarkEnd w:id="22"/&gt;&lt;w:bookmarkEnd w:id="23"/&gt;&lt;w:bookmarkEnd w:id="24"/&gt;&lt;w:bookmarkEnd w:id="25"/&gt;&lt;w:bookmarkEnd w:id="26"/&gt;&lt;w:bookmarkEnd w:id="27"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;22. Сведения о госпитализациях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="9645" w:type="dxa"/&gt;&lt;w:tblInd w:w="62" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="75" w:type="dxa"/&gt;&lt;w:left w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="75" w:type="dxa"/&gt;&lt;w:right w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="2035"/&gt;&lt;w:gridCol w:w="2788"/&gt;&lt;w:gridCol w:w="4822"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2034" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата поступления и выписки&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2786" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Медицинская организация, в которой была оказана мед&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;омощь в стационарных условиях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4819" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заключительный клинический диагноз&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2034" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2786" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4819" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="28" w:name="Par482"/&gt;&lt;w:bookmarkEnd w:id="28"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="29" w:name="Par504"/&gt;&lt;w:bookmarkEnd w:id="29"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;23.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Лист учета доз облучения при рентгенологических исследованиях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="9645" w:type="dxa"/&gt;&lt;w:tblInd w:w="62" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="75" w:type="dxa"/&gt;&lt;w:left w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="75" w:type="dxa"/&gt;&lt;w:right w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="2133"/&gt;&lt;w:gridCol w:w="5070"/&gt;&lt;w:gridCol w:w="2442"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2132" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата проведения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5067" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Название рентгенологического исследования&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2440" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Доза облучения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2132" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5067" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2440" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00453504" w:rsidRPr="00C675B3" w:rsidRDefault="00587921" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00453504" w:rsidRPr="00C675B3" w:rsidSect="00626937"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>False</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblpPr w:leftFromText="180" w:rightFromText="180" w:vertAnchor="text" w:horzAnchor="margin" w:tblpY="-142"/&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="4580"/&gt;&lt;w:gridCol w:w="1488"/&gt;&lt;w:gridCol w:w="3984"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="00FA0372"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="1164"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4580" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00C675B3" w:rsidRPr="00626937" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Наименование медицинской организации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00FA0372" w:rsidRPr="00FA0372" w:rsidRDefault="005B5833" w:rsidP="00FA0372"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1488" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3984" w:type="dxa"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Код формы по ОКУД __________                                        Код организации по ОКПО: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgOKPO&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Медицинская документация                                               Учетная форма N &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;025/у&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Утверждена&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; приказом Минздрава России                                  от 15 декабря 2014 г. N 834н&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="005B5833"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="Par64"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                         &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="1" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="1"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;МЕДИЦИНСКАЯ КАРТА&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00A26A7A" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПАЦИЕНТА, ПОЛУЧАЮЩЕГО МЕДИЦИНСКУЮ ПОМОЩЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;В АМБУЛАТОРНЫХ УСЛОВИЯХ N &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CardNumber&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="2" w:name="Par68"/&gt;&lt;w:bookmarkEnd w:id="2"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1. Дата заполнения медицинской карты: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CardDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="3" w:name="Par69"/&gt;&lt;w:bookmarkEnd w:id="3"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2. Фамилия, имя, отчество: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFIO&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3. Пол: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Gender&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;4. Дата рождения: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BirthDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;5. Место регистрации: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Address&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;; тел.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContactPhone&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="4" w:name="Par74"/&gt;&lt;w:bookmarkEnd w:id="4"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;6. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Местность&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;: Registration&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00A77D4D" w:rsidRPr="00557D8F" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="5" w:name="Par75"/&gt;&lt;w:bookmarkEnd w:id="5"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;InsuranceDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00557D8F" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;8. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;СНИЛС&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="6" w:name="Par76"/&gt;&lt;w:bookmarkEnd w:id="6"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;SNILS&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9. Наимено&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;вание страховой медицинской организации: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;InsuranceCompany&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="7" w:name="Par77"/&gt;&lt;w:bookmarkEnd w:id="7"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;10. Код категории льготы: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BenefitCode&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;11.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Документ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; льготы&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BenefitDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="8" w:name="Par78"/&gt;&lt;w:bookmarkStart w:id="9" w:name="Par111"/&gt;&lt;w:bookmarkStart w:id="10" w:name="Par113"/&gt;&lt;w:bookmarkEnd w:id="8"/&gt;&lt;w:bookmarkEnd w:id="9"/&gt;&lt;w:bookmarkEnd w:id="10"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;12. Семейное положение: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;MaritalStatus&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="11" w:name="Par115"/&gt;&lt;w:bookmarkEnd w:id="11"/&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;13.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Образование: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Education&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="12" w:name="Par117"/&gt;&lt;w:bookmarkEnd w:id="12"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;14. Занятость: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Employment&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;15.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Место работы, должность: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00557D8F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Business&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="13" w:name="Par120"/&gt;&lt;w:bookmarkEnd w:id="13"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;16. Инвалидность: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Disability&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001230CA" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="14" w:name="Par121"/&gt;&lt;w:bookmarkEnd w:id="14"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;17. Группа крови: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BloodGroup&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;18. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Rh&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;-фактор: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;BloodRh&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00715612" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="009F611F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;19. Аллергические реакции: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Allergy&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="15" w:name="Par124"/&gt;&lt;w:bookmarkStart w:id="16" w:name="Par151"/&gt;&lt;w:bookmarkEnd w:id="15"/&gt;&lt;w:bookmarkEnd w:id="16"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:sectPr w:rsidR="001F2DC7" w:rsidRPr="00C675B3"&gt;&lt;w:pgSz w:w="11907" w:h="8391" w:orient="landscape"/&gt;&lt;w:pgMar w:top="567" w:right="851" w:bottom="284" w:left="851" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="720"/&gt;&lt;/w:sectPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="17" w:name="Par154"/&gt;&lt;w:bookmarkStart w:id="18" w:name="Par156"/&gt;&lt;w:bookmarkStart w:id="19" w:name="Par328"/&gt;&lt;w:bookmarkStart w:id="20" w:name="Par330"/&gt;&lt;w:bookmarkStart w:id="21" w:name="Par360"/&gt;&lt;w:bookmarkStart w:id="22" w:name="Par392"/&gt;&lt;w:bookmarkStart w:id="23" w:name="Par427"/&gt;&lt;w:bookmarkStart w:id="24" w:name="Par459"/&gt;&lt;w:bookmarkStart w:id="25" w:name="Par461"/&gt;&lt;w:bookmarkEnd w:id="17"/&gt;&lt;w:bookmarkEnd w:id="18"/&gt;&lt;w:bookmarkEnd w:id="19"/&gt;&lt;w:bookmarkEnd w:id="20"/&gt;&lt;w:bookmarkEnd w:id="21"/&gt;&lt;w:bookmarkEnd w:id="22"/&gt;&lt;w:bookmarkEnd w:id="23"/&gt;&lt;w:bookmarkEnd w:id="24"/&gt;&lt;w:bookmarkEnd w:id="25"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;22. Сведения о госпитализациях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="9645" w:type="dxa"/&gt;&lt;w:tblInd w:w="62" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="75" w:type="dxa"/&gt;&lt;w:left w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="75" w:type="dxa"/&gt;&lt;w:right w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="2035"/&gt;&lt;w:gridCol w:w="2788"/&gt;&lt;w:gridCol w:w="4822"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2034" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата поступления и выписки&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2786" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Медицинская организация, в которой была оказана &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мед&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;омощь в стационарных условиях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4819" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заключительный клинический диагноз&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2034" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2786" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4819" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;hospdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="26" w:name="Par482"/&gt;&lt;w:bookmarkEnd w:id="26"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00B378A5" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="27" w:name="Par504"/&gt;&lt;w:bookmarkEnd w:id="27"/&gt;&lt;w:r w:rsidRPr="00B378A5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;23. Лист учета доз облучения при рентгенологических исследованиях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="9645" w:type="dxa"/&gt;&lt;w:tblInd w:w="62" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="75" w:type="dxa"/&gt;&lt;w:left w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="75" w:type="dxa"/&gt;&lt;w:right w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="2133"/&gt;&lt;w:gridCol w:w="5070"/&gt;&lt;w:gridCol w:w="2442"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2132" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата проведения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5067" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Название рентгенологического исследования&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2440" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Доза облучения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidTr="001F2DC7"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2132" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5067" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2440" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:tcMar&gt;&lt;w:top w:w="102" w:type="dxa"/&gt;&lt;w:left w:w="62" w:type="dxa"/&gt;&lt;w:bottom w:w="102" w:type="dxa"/&gt;&lt;w:right w:w="62" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:hideMark/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C675B3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;radiationdata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="001F2DC7" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00453504" w:rsidRPr="00C675B3" w:rsidRDefault="005B5833" w:rsidP="00C675B3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Courier New" w:hAnsi="Courier New" w:cs="Courier New"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00453504" w:rsidRPr="00C675B3" w:rsidSect="00626937"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>PayContract</x:t>
@@ -66,12 +60,51 @@
   </x:si>
   <x:si>
     <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
-&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="13"/&gt;&lt;w:szCs w:val="13"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ДОГОВОР № &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractNumber&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;         &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                             &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на предоставление платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;г. Москва    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;                                                               «__» _______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__ 20&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="709"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;), далее по тексту – «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;», в лице директора обособленного структурного подразделения  - &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0066798E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0066798E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DirectorGenitive&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, действующей на основании Доверенности от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PayContractLicense&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, с одной стороны, и родитель (законный представитель), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;именуемый в дальнейшем «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;»,&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="709"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________________________________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Фамилия, Имя, Отчество, степень родства &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;родителя (законного представителя) ребенка)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;действующий&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ая&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) в интересах ребенка, именуемого в дальнейшем «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;»,&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00E612D8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______________________________________________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Фамилия, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Имя, Отчество, ребенка, дата рождения)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;с другой стороны, заключили настоящий Договор о нижеследующем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1. Предмет Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1.1. Исполнитель обязуется предоставить пациенту платные  медицинские услуги &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="10215"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidTr="006D7491"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="10421" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(далее по тексту – медицинские услуги) в обособленном структурном подразделении Исполнителя – &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(далее по тексту – Институт), расположенном по адресу:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, а Заказчик оплатить оказанные Исполнителем медицинские услуги в порядке, установленно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;м настоящим Договором.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1.2. Медицинские услуги предоставляются с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractBeginDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; по &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractEndDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в соответствии с требованиями, установленными для оказания медицинских услуг на территории Российской Федерации&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1.3. До заключения настоящего договора За&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;казчику разъяснено, что несоблюдение указаний (рекомендаций) Исполнителя (медицинских работников, предоставляющих медицинскую услугу), в том числе назначенного режима лечения, могут снизить качество предоставляемой платной медицинской услуги, повлечь за со&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;бой невозможность ее завершения в срок или отрицательно сказаться на состоянии здоровья Пациента.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1.4. Исполнителем доведена до сведения Заказчика информация о порядке оказания медицинских услуг в рамках Программы государственных гарантий оказания граждана&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;м РФ. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заключая настоящий договор, Заказчик проинформирован о том, что Пациент имеет право на бесплатную медицинскую помощь согласно ч.1 ст.41 Конституции РФ и может реализовать это право через Программу государственных гарантий оказания гражданам РФ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;бесплатной медицинской помощи; что при определении размера налоговой базы Заказчик имеет право на получение социальных налоговых вычетов в соответствии со ст.219 п.3 Налогового кодекса РФ в сумме, уплаченной в налоговом периоде за услуги по лечению Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;а, предоставленные Заказчику Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2. Стоимость медицинских услуг, сроки предоставления и порядок их оплаты&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2.1. Стоимость и сроки оказания медицинских услуг, предоставляемых по договору, указаны в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="00DB12F0" w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Приложение&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="00DB12F0" w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; № 1 к настоящему договору&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;являющемся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; неотъемлемой частью Догов&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Оплата медицинских услуг производится в соответствии с действующим на день оплаты Прейскурантом, путем внесения денежных средств Заказчиком в кассу Исполнителя в размере 100% предоплаты, с выдачей Заказчику контрольно-кассового чека и документов &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;установленного образца, подтверждающих произведенную оплату медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2.3&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;. Возврат денежных средств Заказчику производится в соответствии с кассовой дисциплиной Исполнителя:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- в случае отказа Заказчика от услуги при условии, если услуга уже оплаче&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- в случае возникновения форс-мажорных обстоятельств, приведших к невозможности оказания услуги Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3. Права и обязанности Сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.1. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  обязуется:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.1. Предоставить Заказчику&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;доступную и достоверную информацию:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о порядке ока&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;зания и видах медицинских услуг, предоставляемых в Институте;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о видах и стоимости медицинских услуг, оказываемых за плату;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о порядке и сроках оказания платных медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:strike/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.1.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Своевременно оказывать медицинские услуги надлежащего качества в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;соответствии с принятыми технологиями, разрешенным к применению в установленном законом порядке и соответствовать стандартам оказания медицинской помощи, установленным на территории Российской Федерации, а также в соответствии с объективным состоянием Паци&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ента на момент оказания медицинской услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-7"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-7"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.3.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Вести медицинскую документацию Пациента, учетные и отчетные статистические формы при оказании Пациенту медицинских услуг, соблюдать установленные законодательством Российской Федерации требования к &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;оформлению и ведению медицинской документации и учетных и отчетных статистических форм, порядку и срокам их представления.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.4. По завершении оказания услуг выдать Пациенту медицинские документы (копии медицинских документов, выписки из медицинских докум&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ентов), отражающие состояние его здоровья после оказания медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.5. Информировать&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчика об обстоятельствах, которые могут привести к увеличению объема и стоимости, оказываемых Пациенту услуг, о предстоящих Пациенту лечебно-диагностически&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;х мероприятиях, о необходимых медикаментозных препаратах и расходных материалах и их стоимости, возможных осложнениях, которые могут возникнуть в ходе лечения. Изменение плана лечения Пациента согласовывать с Заказчиком, фиксировать в амбулаторной карте и &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в заявлении, подписанном обеими Сторонами.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.6. Ознакомить Заказчика с режимом работы Института, правилами внутреннего распорядка и правилами поведения пациентов и их законных представителей в Клинике Института.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.7.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Соблюдать правила медицинской этики&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,  врачебную тайну и иные сведения конфиденциального характера.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обязуется:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.2.1. Оплатить медицинские услуги в сроки и в порядке, определенные настоящим Договором. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.2. Являться на прием в установленное время.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.3. Сообщать лечащему вр&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ачу о состоянии здоровья Пациента, принимаемых им лекарственных препаратах,  немедленно извещать лечащего врача об изменениях в состоянии здоровья Пациента в процессе лечения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C" w:rsidDel="0051586F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.4. Выполнять все требования, необходимые для организации лечебного процесса&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, и рекомендации лечащего врача.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t xml:space="preserve"&gt;3.2.5. Соблюдать режим работы Института, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Правила внутреннего распорядка и санитарно-эпидемиологического режима Клиники Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, правила поведения Пациентов и их законных представителей&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в Клинике Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; .&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.6. Бережно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; относиться к имуществу Исполнителя&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;возместить ущерб, причиненный Пациентом имуществу Исполнителя&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; имеет право:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3.1. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:spacing w:val="-9"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Назначать лечащего врача&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, при отсутствии лечащего врача по об&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ъективным причинам (болезнь, отпуск и т.п.) назначить другого врача для продолжения лечения Пациента.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:spacing w:val="-6"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3.2. Запрашивать у Заказчика сведения и дополнительные документы, и их копии  (в случае предыдущего лечения в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;других лечебных учреждениях), необходимые &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;для эффективного лечения Пациента.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.3.3. Отказаться от оказания услуг, являющихся предметом настоящего Договора, в случае&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- обнаружения нецелесообразности их исполнения;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- при наличии противопоказаний для Пациента;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- если требования Заказчика не соответст&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;вуют требованиям технологий и могут вызвать нежелательные последствия для Пациента;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:strike/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-1"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- невыполнения Пациентом рекомендаций и назначений лечащего врача; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- грубого и систематического нарушения Пациентом правил внутреннего распорядка &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-15"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Клиники Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, режима&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; лечения и правил поведения Пациентов и их законных представителей&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-15"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в Клинике Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- высокой степени риска возможных осложнений.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.4. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; имеет право:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.1. Получать информацию о состоянии здоровья Пациента, ходе обследования и лечения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.4.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Получить  полную и понятную информацию об оказываемых медицинских услугах и их стоимости.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.3. Получить полную и понятную информацию о правилах предоставления медицинских услуг в рамках Программы государственных гарантий.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.4. Свободного выбора специал&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;иста&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(по предварительной записи, лечащего врача).&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.5. Получить сведения о наличии лицензии Заказчика, квалификации, образовании специалистов, оказывающих платные медицинские услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.6.Отказаться от дальнейшего лечения Пациента при условии обязательн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ой оплаты Заказчиком выполненных услуг. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.7. Получать социальные налоговые вычеты в сумме, уплаченной в налоговом периоде за услуги по лечению, предоставленные Пациенту Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.8. Получить у Исполнителя (по требованию) смету на предоставляемые&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинские услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.  Порядок исполнения Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.1. Исполнитель приступает к оказанию медицинских услуг с момента внесения денежных сре&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;дств в к&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ассу Исполнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.2. Медицинские услуги предоставляются при наличии информированного добровольного согла&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;сия Пациента/Законного представителя Пациента, данного в порядке, установленном &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:hyperlink w:anchor="block_20" w:history="1"&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;законодательством&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:hyperlink&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Российской Федерации об охране здоровья граждан.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.3. Медицинские услуги оказываются Институтом Заказчику по предварительной запис&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;и на прием по телефону или в регистратуре,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:iCs/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; а в порядке исключения - вне установленной очереди. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.4. До сведения Заказчика доводится информация о правилах предоставления медицинских услуг, внутреннего распорядка и санитарно-эпидемиологического режима в Ин&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ституте&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;путем ознакомления с ней на стендах Института.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;5. Срок действия Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Настоящий договор вступает в силу с момента его подписания Сторонами и действует в течение одного календарного года.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6. Ответственность Сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.1. Стороны несут ответственн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ость за невыполнение или ненадлежащее выполнение условий настоящего Договора в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.2. Исполнитель несет ответственность за качество выполненных медицинских услуг, достаточных и адекватных состоянию Пацие&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нта на момент обращения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.3. Исполнитель не несет ответственности за результаты и качество оказания медицинских услуг в случаях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- несоблюдения Заказчиком требований, необходимых для организации лечебного процесса, и рекомендаций по лечению;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;несвоевременного сообщения Пациентом/Законным представителем о возникших изменениях в состоянии его здоровья;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- прекращения (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;незавершения&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) лечения Пациента по инициативе Заказчика.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;6.4. Вред, причиненный жизни или здоровью пациента в результате &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;предоставления некачественной медицинской услуги, подлежит возмещению Исполнителем в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;При установлении факта ненадлежащего исполнения Исполнителем обязательств по договору по  соглашению Сторон возможно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - назначение нового срока оказания услуги;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - уменьшение стоимости предоставленной услуги;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - повторное исполнение услуги другим специалистом;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - расторжение договора с возмещением стоимости услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.5. Заказчик несет ответственность:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за достоверност&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ь и полноту предоставленной информации о Пациенте;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за выполнение требований и рекомендаций врача.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за своевременность и полноту оплаты медицинских услуг, предоставленных Пациенту.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7. Изменение и расторжение договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7.1. Изменение Договора возможно по&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; соглашению сторон.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7.2. Все изменения и дополнения к настоящему Договору, требующие взаимного согласия Сторон, будут действительны только при условии, если они совершены в письменной форме и подписаны уполномоченными на то представителями Сторон. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;До&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;говор&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; может быть расторгнут досрочно:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- по обоюдному согласию Сторон;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- одной из Сторон в одностороннем порядке в случае систематического и/или грубого нарушения другой стороной условий настоящего Договора с уведомлением о расторжении Договора другой сторо&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ны;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- одной из Сторон  в связи с изменениями законодательства РФ, нормативно-правовых актов Исполнителя;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- Исполнителем в одностороннем порядке в случае прекращения осуществления деятельности, указанной в настоящем Договоре, ликвидации или реорганизации Ис&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;полнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;7.4. Прекращение настоящего Договора освобождает Стороны от исполнения обязательств только после того, как они выполнят свои обязательства, возникшие у них до момента прекращения настоящего Договора, в полном объеме.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;8. Порядок разрешения &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;споров&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;8.1. При возникновении спорных вопросов Стороны принимают все необходимые меры для их урегулирования путем переговоров. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.2. Все претензии по финансовым расчетам, качеству предоставления медицинских услуг и другим вопросам рассматриваются и разреша&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ются по согласованию Сторон. При &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;не достижении&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; согласия споры подлежат рассмотрению в суде с возможным досудебным урегулированием споров в претензионном порядке. Претензия подается Стороной в письменной форме и должна быть рассмотрена противоположной Сторо&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ной в 10-дневный срок со дня ее получения, по итогам рассмотрения претензии Стороне, подавшей ее, незамедлительно направляется ответ. В случае неполучения ответа на претензию в течение 30 дней со дня ее направления Сторона, подавшая претензию, вправе обрат&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;иться в суд за защитой своих нарушенных прав.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.3. Во всем остальном, что не предусмотрено настоящим договором, Стороны руководствуются законодательством РФ.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9. Заключительные положения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.1. Медицинские услуги предоставляются Исполнителем в соответствии с&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;условиями и сроками, определенными настоящим Договором. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.2. Настоящий Договор Заказчик заключил, находясь в здравом уме, ясной памяти и действуя добровольно и осознанно, выбрав порядок оказания услуг, установленный настоящим договором.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.3. Настоящий До&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;говор составлен в двух экземплярах, имеющих равную юридическую силу, по одному экземпляру для Заказчика и Исполнителя.  Заявления  являются неотъемлемой частью настоящего Договора и составляются в двух экземплярах, имеющих равную юридическую силу, по одном&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;у экземпляру для Заказчика и Исполнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10. Прочие условия&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10.1. Любые условия, не оговоренные настоящим Договором, рассматриваются Сторонами в соответствии с действующим законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;10.2. В случае если при предоставлении &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;медицинских услуг потребуется предоставление дополнительных медицинских услуг по экстренным показаниям для устранения угрозы жизни Пациента при внезапных острых заболеваниях, состояниях, обострениях хронических заболеваний, такие медицинские услуги оказыва&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ются без взимания платы в соответствии с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:hyperlink w:history="1"&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Федеральным законом&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:hyperlink&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; "Об основах охраны здоровья граждан в Российской Федерации".&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="10215"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="007878A8"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="10421" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="007878A8"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="007878A8" w:rsidRDefault="00C6544A" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;подтверждаю, что мое желание получить платные медицинские услуги является добровольным, и я проинформирован  о возможности получения бесплатных медицинских услуг в обособленном структурном подразделении Исполнителя – &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="007914AE" w:rsidRDefault="00C6544A" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKINameGenitive&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="007914AE"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________ (подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПОДПИСИ  СТОРОН&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="4468"/&gt;&lt;w:gridCol w:w="5747"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заказчик &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge w:val="restart"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Юридический адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="001D466B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес оказания услуг: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="001D466B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Тел.(495) 484-02-92; факс: (495) 483-33-35&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Ф.И.О. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Паспортные данные: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientPassport&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="007878A8" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="00E612D8" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Директор обособленного структурного подразделения   &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ______________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DirectorShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="00747EF5" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Родитель  (законный  представитель)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="001D466B" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="51"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="007878A8"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«___» ____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;____ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;20_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«___ » ______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____ 20&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00C6544A" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00C6544A" w:rsidP="004A6711"/&gt;&lt;w:p w:rsidR="009B084F" w:rsidRDefault="00C6544A"&gt;&lt;w:r&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="2123"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;Приложение №1&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="2123"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                                                                        к Договору на оказание платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                     (для физических лиц)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="540"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;от  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«____»__________________ 20_____г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ПЕРЕЧЕНЬ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;оказываемых платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DB12F0" w:rsidRPr="00DB12F0" w:rsidRDefault="00DB12F0" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;период&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;с&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractBeginDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; по &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractEndDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="55" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="55" w:type="dxa"/&gt;&lt;w:left w:w="55" w:type="dxa"/&gt;&lt;w:bottom w:w="55" w:type="dxa"/&gt;&lt;w:right w:w="55" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="0000" w:firstRow="0" w:lastRow="0" w:firstColumn="0" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="749"/&gt;&lt;w:gridCol w:w="7215"/&gt;&lt;w:gridCol w:w="2143"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="749" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7215" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Медицинские услуги&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Стоимость&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="749" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7215" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7964" w:type="dxa"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ИТОГО&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00DB12F0" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;TotalSum&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подписи сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;C&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пециалист&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик/&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00C6544A" w:rsidP="00C6544A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;_____________________/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C6544A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4248" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;подпись&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4956" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;*__________________/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4956" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;подпись &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;*&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, достигший 14-летнего возраста&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00C6544A" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00E2514E" w:rsidRPr="004A6711" w:rsidRDefault="00C6544A" w:rsidP="004A6711"/&gt;&lt;w:sectPr w:rsidR="00E2514E" w:rsidRPr="004A6711" w:rsidSect="00086A54"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="397" w:right="567" w:bottom="397" w:left="1134" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="13"/&gt;&lt;w:szCs w:val="13"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ДОГОВОР № &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractNumber&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;         &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                             &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на предоставление платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;г. Москва    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;                                                               «__» _______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__ 20&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="709"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;), далее по тексту – «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;», в лице директора обособленного структурного подразделения  -&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00326C83"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DirectorGenitive&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, действующей на основании Доверенности от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PayContractLicense&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, с одной стороны, и родитель (законный представитель), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;именуемый в дальнейшем «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;»,&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="709"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________________________________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Фамилия, Имя, Отчество, степень родства &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;родителя (законного представителя) ребенка)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;действующий&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ая&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) в интересах ребенка, именуемого в дальнейшем «&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;»,&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00E612D8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______________________________________________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Фамилия, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Имя, Отчество, ребенка, дата рождения)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="333333"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;с другой стороны, заключили настоящий Договор о нижеследующем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1. Предмет Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1.1. Исполнитель обязуется предоставить пациенту платные  медицинские услуги &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="10215"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="10421" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(далее по тексту – медицинские услуги) в обособленном структур&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ном подразделении Исполнителя –&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00326C83"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(далее по тексту – Инс&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;титут), расположенном по адресу&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00326C83"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, а Заказчик оплатить оказанные Исполнителем медицинские услуги в порядке, установленно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;м настоящим Договором.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;1.2. Медицинские услуги предоставляются с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractBeginDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; по &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractEndDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в соответствии с требованиями, установленными для оказания медицинских услуг на территории Российской Федерации&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1.3. До заключения настоящего договора За&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;казчику разъяснено, что несоблюдение указаний (рекомендаций) Исполнителя (медицинских работников, предоставляющих медицинскую услугу), в том числе назначенного режима лечения, могут снизить качество предоставляемой платной медицинской услуги, повлечь за со&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;бой невозможность ее завершения в срок или отрицательно сказаться на состоянии здоровья Пациента.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1.4. Исполнителем доведена до сведения Заказчика информация о порядке оказания медицинских услуг в рамках Программы государственных гарантий оказания граждана&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;м РФ. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заключая настоящий договор, Заказчик проинформирован о том, что Пациент имеет право на бесплатную медицинскую помощь согласно ч.1 ст.41 Конституции РФ и может реализовать это право через Программу государственных гарантий оказания гражданам РФ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;бесплатной медицинской помощи; что при определении размера налоговой базы Заказчик имеет право на получение социальных налоговых вычетов в соответствии со ст.219 п.3 Налогового кодекса РФ в сумме, уплаченной в налоговом периоде за услуги по лечению Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;а, предоставленные Заказчику Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2. Стоимость медицинских услуг, сроки предоставления и порядок их оплаты&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2.1. Стоимость и сроки оказания медицинских услуг, предоставляемых по договору, указаны в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Приложение № 1 к настоящему договору&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;являющемс&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;я&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; неотъемлемой частью Договора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оплата медицинских услуг производится в соответствии с действующим на день оплаты Прейскурантом, путем внесения денежных средств Заказчиком в кассу Исполнителя в размере 100% предоплаты, с выдачей Заказчику контрольно-к&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ассового чека и документов установленного образца, подтверждающих произведенную оплату медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2.3&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;. Возврат денежных средств Заказчику производится в соответствии с кассовой дисциплиной Исполнителя:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- в случае отказа Заказчика от услуги при усло&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;вии, если услуга уже оплачена;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- в случае возникновения форс-мажорных обстоятельств, приведших к невозможности оказания услуги Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3. Права и обязанности Сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.1. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  обязуется:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.1. Предоставить Заказчику&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;доступную и достоверную и&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нформацию:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о порядке оказания и видах медицинских услуг, предоставляемых в Институте;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о видах и стоимости медицинских услуг, оказываемых за плату;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - о порядке и сроках оказания платных медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:strike/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.1.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Своевременно оказывать медицинские услуги надлежащего качества в соответствии с принятыми технологиями, разрешенным к применению в установленном законом порядке и соответствовать стандартам оказания медицинской помощи, установленным на территории Российско&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;й Федерации, а также в соответствии с объективным состоянием Пациента на момент оказания медицинской услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-7"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-7"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.3.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Вести медицинскую документацию Пациента, учетные и отчетные статистические формы при оказании Пациенту медицинских услуг, соблюдать установленные законодательством Российской Федерации требования к оформлению и ведению медицинской документации и учетных и&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; отчетных статистических форм, порядку и срокам их представления.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.1.4. По завершении оказания услуг выдать Пациенту медицинские документы (копии медицинских документов, выписки из медицинских документов), отражающие состояние его здоровья после оказания &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;медицинских услуг.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.5. Информировать&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="FF00FF"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заказчика об обстоятельствах, которые могут привести к увеличению объема и стоимости, оказываемых Пациенту услуг, о предстоящих Пациенту лечебно-диагностических мероприятиях, о необходимых медикаментозных препаратах &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;и расходных материалах и их стоимости, возможных осложнениях, которые могут возникнуть в ходе лечения. Изменение плана лечения Пациента согласовывать с Заказчиком, фиксировать в амбулаторной карте и в заявлении, подписанном обеими Сторонами.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.6. Ознаком&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ить Заказчика с режимом работы Института, правилами внутреннего распорядка и правилами поведения пациентов и их законных представителей в Клинике Института.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.1.7.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Соблюдать правила медицинской этики,  врачебную тайну и иные сведения конфиденциального хара&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ктера.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обязуется:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.2.1. Оплатить медицинские услуги в сроки и в порядке, определенные настоящим Договором. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.2. Являться на прием в установленное время.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.3. Сообщать лечащему врачу о состоянии здоровья Пациента, принимаемых им лекарст&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;венных препаратах,  немедленно извещать лечащего врача об изменениях в состоянии здоровья Пациента в процессе лечения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C" w:rsidDel="0051586F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.4. Выполнять все требования, необходимые для организации лечебного процесса, и рекомендации лечащего врача.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="009941C6" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t xml:space="preserve"&gt;3.2.5. Соблюдать режим работы Института, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Правила внутреннего распорядка и санитарно-эпидемиологического режима Клиники Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, правила поведения Пациентов и их законных представителей&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в Клинике Института .&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.2.6. Бережно относиться к имуществу Исполните&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ля&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;возместить ущерб, причиненный Пациентом имуществу Исполнителя&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; имеет право:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3.1. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:spacing w:val="-9"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Назначать лечащего врача&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, при отсутствии лечащего врача по объективным причинам (болезнь, отпу&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ск и т.п.) назначить другого врача для продолжения лечения Пациента.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:spacing w:val="-6"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.3.2. Запрашивать у Заказчика сведения и дополнительные документы, и их копии  (в случае предыдущего лечения в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;других лечебных учреждениях), необходимые для эффективного лечения Пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.3.3. Отказаться от оказания услуг, являющихся предметом настоящего Договора, в случае&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- обнаружения нецелесообразности их исполнения;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- при наличии противопоказаний для Пациента;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- если требования Заказчика не соответствуют требованиям технологий и мог&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ут вызвать нежелательные последствия для Пациента;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:strike/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-1"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- невыполнения Пациентом рекомендаций и назначений лечащего врача; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- грубого и систематического нарушения Пациентом правил внутреннего распорядка &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-15"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Клиники Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, режима&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; лечения и правил поведения Пациентов и их законных представителей&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:spacing w:val="-15"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; в Клинике Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- высокой степени риска возможных осложнений.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.4. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; имеет право:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.1. Получать информацию о состоянии здоровья Пациента, ходе обследования и лечения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;3.4.2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Получить  полную и понятную информацию об оказываемых медицинских услугах и их стоимости.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.3. Получить полную и понятную информацию о правилах предоставления медицинских услуг в рамках Программы государственных гарантий.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.4. Свободного выбора специал&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;иста&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009941C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(по предварительной записи, лечащего врача).&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.5. Получить сведения о наличии лицензии Заказчика, квалификации, образовании специалистов, оказывающих платные медицинские услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.6.Отказаться от дальнейшего лечения Пациента при условии обязательн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ой оплаты Заказчиком выполненных услуг. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.7. Получать социальные налоговые вычеты в сумме, уплаченной в налоговом периоде за услуги по лечению, предоставленные Пациенту Исполнителем.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3.4.8. Получить у Исполнителя (по требованию) смету на предоставляемые&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинские услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.  Порядок исполнения Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.1. Исполнитель приступает к оказанию медицинских услуг с момента внесения денежных сре&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;дств в к&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ассу Исполнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.2. Медицинские услуги предоставляются при наличии информированного добровольного согла&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;сия Пациента/Законного представителя Пациента, данного в порядке, установленном &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:hyperlink w:anchor="block_20" w:history="1"&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;законодательством&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:hyperlink&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Российской Федерации об охране здоровья граждан.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.3. Медицинские услуги оказываются Институтом Заказчику по предварительной запис&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;и на прием по телефону или в регистратуре,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:iCs/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; а в порядке исключения - вне установленной очереди. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.4. До сведения Заказчика доводится информация о правилах предоставления медицинских услуг, внутреннего распорядка и санитарно-эпидемиологического режима в Ин&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ституте&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;путем ознакомления с ней на стендах Института.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;5. Срок действия Договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Настоящий договор вступает в силу с момента его подписания Сторонами и действует в течение одного календарного года.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6. Ответственность Сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.1. Стороны несут ответственн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ость за невыполнение или ненадлежащее выполнение условий настоящего Договора в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.2. Исполнитель несет ответственность за качество выполненных медицинских услуг, достаточных и адекватных состоянию Пацие&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нта на момент обращения.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.3. Исполнитель не несет ответственности за результаты и качество оказания медицинских услуг в случаях&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- несоблюдения Заказчиком требований, необходимых для организации лечебного процесса, и рекомендаций по лечению;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;- &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;несвоевременного сообщения Пациентом/Законным представителем о возникших изменениях в состоянии его здоровья;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- прекращения (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;незавершения&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) лечения Пациента по инициативе Заказчика.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.4. Вред, причиненный жизни или здоровью пациента в результате предоставле&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ния некачественной медицинской услуги, подлежит возмещению Исполнителем в соответствии с законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;При установлении факта ненадлежащего исполнения Исполнителем обязательств по договору по  соглашению Сторон возможно:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - назнач&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ение нового срока оказания услуги;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - уменьшение стоимости предоставленной услуги;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - повторное исполнение услуги другим специалистом;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; - расторжение договора с возмещением стоимости услуги.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.5. Заказчик несет ответственность:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за достоверность и полноту&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; предоставленной информации о Пациенте;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за выполнение требований и рекомендаций врача.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- за своевременность и полноту оплаты медицинских услуг, предоставленных Пациенту.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7. Изменение и расторжение договора&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7.1. Изменение Договора возможно по соглашению&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; сторон.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7.2. Все изменения и дополнения к настоящему Договору, требующие взаимного согласия Сторон, будут действительны только при условии, если они совершены в письменной форме и подписаны уполномоченными на то представителями Сторон. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;7.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Договор&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; может&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; быть расторгнут досрочно:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- по обоюдному согласию Сторон;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- одной из Сторон в одностороннем порядке в случае систематического и/или грубого нарушения другой стороной условий настоящего Договора с уведомлением о расторжении Договора другой стороны;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- одной&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; из Сторон  в связи с изменениями законодательства РФ, нормативно-правовых актов Исполнителя;&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;- Исполнителем в одностороннем порядке в случае прекращения осуществления деятельности, указанной в настоящем Договоре, ликвидации или реорганизации Исполнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:widowControl w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;7.4. Прекращение настоящего Договора освобождает Стороны от исполнения обязательств только после того, как они выполнят свои обязательства, возникшие у них до момента прекращения настоящего Договора, в полном объеме.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8. Порядок разрешения споров&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;8.1. При возникновении спорных вопросов Стороны принимают все необходимые меры для их урегулирования путем переговоров. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.2. Все претензии по финансовым расчетам, качеству предоставления медицинских услуг и другим вопросам рассматриваются и разрешаются по&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; согласованию Сторон. При &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;не достижении&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; согласия споры подлежат рассмотрению в суде с возможным досудебным урегулированием споров в претензионном порядке. Претензия подается Стороной в письменной форме и должна быть рассмотрена противоположной Стороной в 1&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;0-дневный срок со дня ее получения, по итогам рассмотрения претензии Стороне, подавшей ее, незамедлительно направляется ответ. В случае неполучения ответа на претензию в течение 30 дней со дня ее направления Сторона, подавшая претензию, вправе обратиться в&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; суд за защитой своих нарушенных прав.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:autoSpaceDN w:val="0"/&gt;&lt;w:adjustRightInd w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:outlineLvl w:val="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.3. Во всем остальном, что не предусмотрено настоящим договором, Стороны руководствуются законодательством РФ.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9. Заключительные положения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.1. Медицинские услуги предоставляются Исполнителем в соответствии с&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;условиями и сроками, определенными настоящим Договором. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.2. Настоящий Договор Заказчик заключил, находясь в здравом уме, ясной памяти и действуя добровольно и осознанно, выбрав порядок оказания услуг, установленный настоящим договором.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8.3. Настоящий Дог&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;овор составлен в двух экземплярах, имеющих равную юридическую силу, по одному экземпляру для Заказчика и Исполнителя.  Заявления  являются неотъемлемой частью настоящего Договора и составляются в двух экземплярах, имеющих равную юридическую силу, по одному&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; экземпляру для Заказчика и Исполнителя.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10. Прочие условия&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10.1. Любые условия, не оговоренные настоящим Договором, рассматриваются Сторонами в соответствии с действующим законодательством Российской Федерации.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10.2. В случае если при предоставлении меди&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;цинских услуг потребуется предоставление дополнительных медицинских услуг по экстренным показаниям для устранения угрозы жизни Пациента при внезапных острых заболеваниях, состояниях, обострениях хронических заболеваний, такие медицинские услуги оказываются&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; без взимания платы в соответствии с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:hyperlink w:history="1"&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Федеральным законом&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:hyperlink&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; "Об основах охраны здоровья граждан в Российской Федерации".&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="10215"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="007878A8"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="10421" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="007878A8"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;.3. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заказчик:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="007878A8" w:rsidRDefault="00326C83" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;подтверждаю, что мое желание получить платные медицинские услуги является добровольным, и я проинформирован  о возможности получения бесплатных медицинских услуг в обособленном структурном подразделении Исполнителя – &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="007914AE" w:rsidRDefault="00326C83" w:rsidP="007914AE"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgNameGenitive&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="007914AE"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________ (подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПОДПИСИ  СТОРОН&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="00A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="4468"/&gt;&lt;w:gridCol w:w="5747"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исполнитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заказчик &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge w:val="restart"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Юридический адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="001D466B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00326C83" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес оказания услуг: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Тел.(495) 484-02-92; факс: (495) 483-33-35&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Ф.И.О. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Паспортные данные: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00747EF5" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientPassport&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="97"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;w:vMerge/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="007878A8" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="00E612D8" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Директор обособленного структурного подразделения   &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00326C83" w:rsidRPr="00326C83" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ______________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00747EF5"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DirectorShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007878A8" w:rsidRPr="00747EF5" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Родитель  (законный  представитель)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="001D466B" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidTr="006D7491"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="51"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4468" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="007878A8"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«___» ____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;____ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;20_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5747" w:type="dxa"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="006D7491"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«___ » ______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____ 20&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00770F5C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRPr="00770F5C" w:rsidRDefault="00326C83" w:rsidP="004A6711"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="004A6711" w:rsidRDefault="00326C83" w:rsidP="004A6711"/&gt;&lt;w:p w:rsidR="009B084F" w:rsidRDefault="00326C83"&gt;&lt;w:r&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="2123"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;Приложение №1&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="2123"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                                                                        к Договору на оказание платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                     (для физических лиц)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="540"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;от  «____»__________________ 20_____г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ПЕРЕЧЕНЬ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;оказываемых платных медицинских услуг&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DB12F0" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;период&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;с&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractBeginDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; по &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ContractEnd&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Date&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00326C83" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="55" w:type="dxa"/&gt;&lt;w:tblLayout w:type="fixed"/&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="55" w:type="dxa"/&gt;&lt;w:left w:w="55" w:type="dxa"/&gt;&lt;w:bottom w:w="55" w:type="dxa"/&gt;&lt;w:right w:w="55" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="0000" w:firstRow="0" w:lastRow="0" w:firstColumn="0" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="749"/&gt;&lt;w:gridCol w:w="7215"/&gt;&lt;w:gridCol w:w="2143"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="749" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7215" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Медицинские услуги&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Стоимость&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="749" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7215" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tbldata&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidTr="00AC1C32"&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="20"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="7964" w:type="dxa"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ИТОГО&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2143" w:type="dxa"/&gt;&lt;w:tcBorders&gt;&lt;w:left w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:bottom w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;w:right w:val="single" w:sz="1" w:space="0" w:color="000000"/&gt;&lt;/w:tcBorders&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;TotalSum&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подписи сторон&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;C&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пециалист&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;Заказчик/Пациент&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00326C83" w:rsidP="00C6544A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________  / ________________________  /&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;_____________________/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C6544A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4248" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;подпись&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4956" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Пациент*__________________/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientShortName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00C6544A" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="4956" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;подпись &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="3540" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DB12F0"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;*Пациент, достигший 14-летнего возраста&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009B084F" w:rsidRPr="00DB12F0" w:rsidRDefault="00326C83" w:rsidP="00DB12F0"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00E2514E" w:rsidRPr="004A6711" w:rsidRDefault="00326C83" w:rsidP="004A6711"/&gt;&lt;w:sectPr w:rsidR="00E2514E" w:rsidRPr="004A6711" w:rsidSect="00086A54"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="397" w:right="567" w:bottom="397" w:left="1134" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AgreementMedicalIntervention</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Согласие на медицинское вмешательство</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ИНФОРМИРОВАННОЕ ДОБРОВОЛЬНОЕ СОГЛАСИЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НА МЕДИЦИНСКОЕ ВМЕШАТЕЛЬСТВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="10"/&gt;&lt;w:szCs w:val="10"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00830DEA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Я, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нижеподписавшийся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;аяся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обратившись за получением медицинских услуг в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;обособленное структурное подразделение –&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="008545E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;,   в соответствии с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Приказом МЗ СР РФ от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;23.04.2012 г. N 390-н&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; даю согласие на проведение&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; пациенту &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                  &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;при необходимости следующих вмешательств: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. Опрос, в том числе выявление жалоб, сбор анамнеза. 2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Осмотр, в том числе пальпация, перкуссия, аускультация, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;риноскопия, фарингоскопия, непрямая ларингоскопия, вагинальное исследование (для женщин). 3.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Антропометрические исследования; 4. Термометрия; 5. Тонометрия. 6. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Неинвазивные&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования органа зрения и зрительных функций. 7. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Неинвазивные&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования орган&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;а слуха и слуховых функций. 8. Исследование функций нервной системы (чувствительной и двигательной сферы). 9. Лабораторные методы обследования, в том числе клинические, биохимические, бактериологические, вирусологические, иммунологические (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;со&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; взятием крови&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; из пальца и вены). 10. Функциональные методы обследования, в том числе электрокардиография (ЭКГ), суточное &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мониторирование&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; артериального давления, суточное &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мониторирование&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; электрокардиограммы, спирография, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пневмотахометрия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пикфлуометрия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;рэоэнцефалографи&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;я&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, электроэнцефалография. 11. Рентгенологические методы обследования, в том числе флюорография (для лиц старше 15 лет) и рентгенография, ультразвуковые исследования, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;допплерографические&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования. 12. Введение лекарственных препаратов по назначению врач&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;а, в том числе внутримышечно, внутривенно, подкожно, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;внутрикожно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;. 13. Медицинский массаж, ЛФК.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я понимаю&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, что во время вмешательства или после него могут появиться непредвиденные ранее неблагоприятные обстоятельства, а также могут возникнуть осложнения. Пр&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;и этом медицинские работники делают все возможное для предотвращения возможных осложнений в соответствии с действующими порядками и стандартами  оказания медицинской помощи. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я предупрежден&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, что невыполнение в полном объёме всех рекомендаций медицинского р&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;аботника может быть причиной осложнений и неблагоприятных последствий медицинского вмешательства.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="10"/&gt;&lt;w:szCs w:val="10"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ПОДПИСЬ: _________________________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt; __________________________________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRDefault="008545E3" w:rsidP="00803FC9"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(пациента старше 15 лет, матери / отца / официального &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;опекуна)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00803FC9" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00803FC9"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПОДПИСЬ ВРАЧА: ____________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;                __________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DA63DE" w:rsidRPr="00803FC9" w:rsidRDefault="008545E3"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00DA63DE" w:rsidRPr="00803FC9" w:rsidSect="00803FC9"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ProvidingConfidentialInformation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Согласие о порядке предоставления конфиденциальной информации</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ДОБРОВОЛЬНОЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ИНФОРМИРОВАННОЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; СОГЛАСИЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;О ПОРЯДКЕ ПРЕДОСТАВЛЕНИЯ КОНФИДЕНЦИАЛЬНОЙ ИНФОРМАЦИИ&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Я &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;РАЗРЕШАЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; / НЕ РАЗРЕШАЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ненужное зачеркнуть&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в соответствии с пунктом 5 части 3 статьи 19 Федерального зако&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на от 21.11.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2011 г. N 323-ФЗ "Об основах охраны здоровья граждан в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;РФ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;" предоставлять сведения о фактах моего обращения за медицинской помощью и состоянии здоровья, диагнозе, в т. ч. через регистратуру, а также в случаях неблагоприятного прогноза развития моего заболев&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ания &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;следующим лицам&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Ф.И.О. полностью,  контактный телефон) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:br/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:br/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О. полностью,  контактный телефон)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______________________      ______________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;               (подпись)                             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;        &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Ф.И.О. пациента &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;старше&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; 15 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;лет или законного представителя пациента младше 15 лет)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператор:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;____ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DA63DE" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00DA63DE" w:rsidRPr="00B9194F" w:rsidSect="00325796"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="851" w:right="737" w:bottom="567" w:left="1361" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
+    <x:t>CommonCommissionsJournal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Общий журнал комиссий</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00675AF5" w:rsidRDefault="00F14FF7" w:rsidP="006E3075"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="006E3075"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRDefault="00F14FF7" w:rsidP="006E3075"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="006E3075"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Журнал комиссий&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="5000" w:type="pct"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideH w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideV w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tblBorders&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="579"/&gt;&lt;w:gridCol w:w="640"/&gt;&lt;w:gridCol w:w="1340"/&gt;&lt;w:gridCol w:w="807"/&gt;&lt;w:gridCol w:w="1334"/&gt;&lt;w:gridCol w:w="1196"/&gt;&lt;w:gridCol w:w="497"/&gt;&lt;w:gridCol w:w="464"/&gt;&lt;w:gridCol w:w="907"/&gt;&lt;w:gridCol w:w="654"/&gt;&lt;w:gridCol w:w="1126"/&gt;&lt;w:gridCol w:w="1369"/&gt;&lt;w:gridCol w:w="968"/&gt;&lt;w:gridCol w:w="1147"/&gt;&lt;w:gridCol w:w="999"/&gt;&lt;w:gridCol w:w="1391"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="00F14FF7" w:rsidRPr="00A321B9" w:rsidTr="008820C2"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="189" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A321B9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№ ком.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="209" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;прот&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="436" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата проведения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="263" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Направил&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="434" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Ф.И.О. пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="389" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата рождения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="162" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Соц. статус&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="134" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Карта&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="295" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Отделение&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="213" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Диагноз&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="366" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Тип комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="445" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Вопрос комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="315" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Решение&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="373" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Рекомендации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="325" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Примечание&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="453" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Состав экспертов&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00F14FF7" w:rsidRPr="00A321B9" w:rsidTr="008820C2"&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="189" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00F14FF7" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="209" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="436" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="263" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="434" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="389" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="162" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="134" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="295" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="213" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="366" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="445" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="315" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="373" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="325" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="453" w:type="pct"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="004E4913" w:rsidRDefault="00F14FF7" w:rsidP="004E4913"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="120" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E4913"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="00A321B9" w:rsidRPr="00A321B9" w:rsidRDefault="00F14FF7" w:rsidP="006E3075"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="006E3075" w:rsidRDefault="00F14FF7" w:rsidP="00A321B9"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="006E3075" w:rsidRDefault="00F14FF7"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="006E3075" w:rsidSect="006E3075"&gt;&lt;w:pgSz w:w="16838" w:h="11906" w:orient="landscape"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
     <x:t>ProcessingPersonalData</x:t>
   </x:si>
   <x:si>
@@ -79,33 +112,124 @@
   </x:si>
   <x:si>
     <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
-&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ДОБРОВОЛЬНОЕ ИНФОРМИРОВАННОЕ СОГЛАСИЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на обработку персональных данных&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нижеподписавшийся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;аяся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientIdentityDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00C026ED"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;RelativeTypeName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ребенка &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Документ, удостоверяющий личность ребенка:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="009954EA" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009954EA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientIdentityDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;В соответствии с требованиями статьи 9 Федерального закона "О персональных данных" от 27.07.2006 N 152-ФЗ, статьи 13 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Федерального закона от 21.11.2011 N 323-ФЗ "Об основах охраны здоровья граждан в РФ"&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПОДТВЕРЖДАЮ СВОЕ СОГЛАСИЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; на обработ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ку &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;обособленным структурным подразделением - &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;NIKIName &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;далее - Оператор&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) моих персональных данных, персональных данных представляемого мной (сына, дочери, опекаемого) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00C026ED"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;включающих: фамилию, имя, отчество, пол, дату рождения, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;адрес места жительства, контактные телефоны, реквизиты паспорта (документа удостоверения личности, в том числе свидетельства о рождении), реквизиты полиса ОМС/ДМС, страховой номер индивидуального лицевого счета в Пенсионном фонде России&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;СНИЛС), место рабо&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ты, учебы, данные о состоянии здоровья, заболеваниях, случаях обращения за медицинской помощью и другую информацию - в медико-профилактических целях, в целях установления медицинского диагноза и оказания медицинских услуг по договору, осуществление иных, с&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;вязанных с этим мероприятий, а также в целях организации внутреннего учета Оператора, при условии сохранения врачебной тайны (или – при условии, что эта обработка осуществляется лицом, уполномоченным Оператором&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; и обязанным сохранять &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;профес&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.т&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;айну&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;). &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;В проце&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ссе оказания Оператором &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мне/представляемому мной ребенку в возрасте до 15 лет&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинских услуг &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПРЕДОСТАВЛЯЮ ПРАВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинским работникам (врачам, среднему медицинскому персоналу) передавать мои персональные данные/персональные данные представляемого мн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ой ребенка в возрасте до 15 лет, в том числе составляющие врачебную тайну, другим должностным лицам Оператора в интересах обследования, лечения и внутреннего учета Оператора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я СОГЛАСЕН (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НА&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; осмотр другими медицинскими работниками и  студентами медицин&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ских вузов/ колледжей исключительно в медицинских, научных или обучающих целях с учетом сохранения врачебной тайны.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПРЕДОСТАВЛЯЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ОПЕРАТОРУ ПРАВО ОСУЩЕСТВЛЯТЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; все действия (операции) с  персональными данными, включая сбор, систематизацию, накопление, хран&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ение, обновление, изменение, использование, передачу (в страховую медицинскую организацию, организацию - заказчика медицинских услуг в рамках заключенных договоров), обезличивание, блокирование, уничтожение.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ОПЕРАТОР ВПРАВЕ ОСУЩЕСТВЛЯТЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; следующие способы обработки персональных данных: на бумажных носителях, в информационных системах персональных данных с использованием и без использования средств автоматизации, а также смешанным способом.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ДАЮ СОГЛАСИЕ / НЕ ДАЮ СОГЛАСИЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нужное подчеркн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;уть, ненужное зачеркнуть&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператору на использование персональных данных в целях информирования меня с помощью средств связи путем пересылки мне SMS-сообщений: напоминание о записи на прием к специалисту или исследование (на указанный мной номер мобильного&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; телефона), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на пересылку информации о состоянии здоровья моего ребенка (результаты дополнительных методов обследования и др.) через незащищенные каналы связи&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (электронная почта), для чего &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;собственноручно пишу адрес электронной почты и телефон&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, на который р&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;азрешаю высылать данные о состоянии здоровья и иные сведения: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C026ED" w:rsidRPr="009954EA" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;E&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;mail&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Телефон:______________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подпись и Ф.И.О.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; субъекта персональных данных        ___________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="708" w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(или его законного представителя) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;____________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;     &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сведения в электронную базу данных внесены:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператор: ________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;__________________             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;           ______________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="708" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;mc:AlternateContent&gt;&lt;mc:Choice Requires="wps"&gt;&lt;w:drawing&gt;&lt;wp:anchor distT="0" distB="0" distL="114300" distR="114300" simplePos="0" relativeHeight="251659264" behindDoc="0" locked="0" layoutInCell="0" allowOverlap="1" wp14:anchorId="3C0011AF" wp14:editId="69B34BCD"&gt;&lt;wp:simplePos x="0" y="0"/&gt;&lt;wp:positionH relativeFrom="column"&gt;&lt;wp:posOffset&gt;4329430&lt;/wp:posOffset&gt;&lt;/wp:positionH&gt;&lt;wp:positionV relativeFrom="paragraph"&gt;&lt;wp:posOffset&gt;116205&lt;/wp:posOffset&gt;&lt;/wp:positionV&gt;&lt;wp:extent cx="215900" cy="215900"/&gt;&lt;wp:effectExtent l="19050" t="19050" r="0" b="0"/&gt;&lt;wp:wrapNone/&gt;&lt;wp:docPr id="2" name="Полилиния 2"/&gt;&lt;wp:cNvGraphicFramePr&gt;&lt;a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/&gt;&lt;/wp:cNvGraphicFramePr&gt;&lt;a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"&gt;&lt;a:graphicData uri="http://schemas.microsoft.com/office/word/2010/wordprocessingShape"&gt;&lt;wps:wsp&gt;&lt;wps:cNvSpPr&gt;&lt;a:spLocks noChangeAspect="1" noChangeArrowheads="1"/&gt;&lt;/wps:cNvSpPr&gt;&lt;wps:spPr bwMode="auto"&gt;&lt;a:xfrm flipH="1"&gt;&lt;a:off x="0" y="0"/&gt;&lt;a:ext cx="215900" cy="215900"/&gt;&lt;/a:xfrm&gt;&lt;a:custGeom&gt;&lt;a:avLst/&gt;&lt;a:gdLst&gt;&lt;a:gd name="G0" fmla="+- 15126 0 0"/&gt;&lt;a:gd name="G1" fmla="+- 2912 0 0"/&gt;&lt;a:gd name="G2" fmla="+- 12158 0 2912"/&gt;&lt;a:gd name="G3" fmla="+- G2 0 2912"/&gt;&lt;a:gd name="G4" fmla="*/ G3 32768 32059"/&gt;&lt;a:gd name="G5" fmla="*/ G4 1 2"/&gt;&lt;a:gd name="G6" fmla="+- 21600 0 15126"/&gt;&lt;a:gd name="G7" fmla="*/ G6 2912 6079"/&gt;&lt;a:gd name="G8" fmla="+- G7 15126 0"/&gt;&lt;a:gd name="T0" fmla="*/ 15126 w 21600"/&gt;&lt;a:gd name="T1" fmla="*/ 0 h 21600"/&gt;&lt;a:gd name="T2" fmla="*/ 15126 w 21600"/&gt;&lt;a:gd name="T3" fmla="*/ 12158 h 21600"/&gt;&lt;a:gd name="T4" fmla="*/ 3237 w 21600"/&gt;&lt;a:gd name="T5" fmla="*/ 21600 h 21600"/&gt;&lt;a:gd name="T6" fmla="*/ 21600 w 21600"/&gt;&lt;a:gd name="T7" fmla="*/ 6079 h 21600"/&gt;&lt;a:gd name="T8" fmla="*/ 17694720 60000 65536"/&gt;&lt;a:gd name="T9" fmla="*/ 5898240 60000 65536"/&gt;&lt;a:gd name="T10" fmla="*/ 5898240 60000 65536"/&gt;&lt;a:gd name="T11" fmla="*/ 0 60000 65536"/&gt;&lt;a:gd name="T12" fmla="*/ 12427 w 21600"/&gt;&lt;a:gd name="T13" fmla="*/ G1 h 21600"/&gt;&lt;a:gd name="T14" fmla="*/ G8 w 21600"/&gt;&lt;a:gd name="T15" fmla="*/ G2 h 21600"/&gt;&lt;/a:gdLst&gt;&lt;a:ahLst/&gt;&lt;a:cxnLst&gt;&lt;a:cxn ang="T8"&gt;&lt;a:pos x="T0" y="T1"/&gt;&lt;/a:cxn&gt;&lt;a:cxn ang="T9"&gt;&lt;a:pos x="T2" y="T3"/&gt;&lt;/a:cxn&gt;&lt;a:cxn ang="T10"&gt;&lt;a:pos x="T4" y="T5"/&gt;&lt;/a:cxn&gt;&lt;a:cxn ang="T11"&gt;&lt;a:pos x="T6" y="T7"/&gt;&lt;/a:cxn&gt;&lt;/a:cxnLst&gt;&lt;a:rect l="T12" t="T13" r="T14" b="T15"/&gt;&lt;a:pathLst&gt;&lt;a:path w="21600" h="21600"&gt;&lt;a:moveTo&gt;&lt;a:pt x="21600" y="6079"/&gt;&lt;/a:moveTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="15126" y="0"/&gt;&lt;/a:lnTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="15126" y="2912"/&gt;&lt;/a:lnTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="12427" y="2912"/&gt;&lt;/a:lnTo&gt;&lt;a:cubicBezTo&gt;&lt;a:pt x="5564" y="2912"/&gt;&lt;a:pt x="0" y="7052"/&gt;&lt;a:pt x="0" y="12158"/&gt;&lt;/a:cubicBezTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="0" y="21600"/&gt;&lt;/a:lnTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="6474" y="21600"/&gt;&lt;/a:lnTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="6474" y="12158"/&gt;&lt;/a:lnTo&gt;&lt;a:cubicBezTo&gt;&lt;a:pt x="6474" y="10550"/&gt;&lt;a:pt x="9139" y="9246"/&gt;&lt;a:pt x="12427" y="9246"/&gt;&lt;/a:cubicBezTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="15126" y="9246"/&gt;&lt;/a:lnTo&gt;&lt;a:lnTo&gt;&lt;a:pt x="15126" y="12158"/&gt;&lt;/a:lnTo&gt;&lt;a:close/&gt;&lt;/a:path&gt;&lt;/a:pathLst&gt;&lt;/a:custGeom&gt;&lt;a:solidFill&gt;&lt;a:srgbClr val="FFFFFF"/&gt;&lt;/a:solidFill&gt;&lt;a:ln w="9525"&gt;&lt;a:solidFill&gt;&lt;a:srgbClr val="000000"/&gt;&lt;/a:solidFill&gt;&lt;a:miter lim="800000"/&gt;&lt;a:headEnd/&gt;&lt;a:tailEnd/&gt;&lt;/a:ln&gt;&lt;/wps:spPr&gt;&lt;wps:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1"&gt;&lt;a:noAutofit/&gt;&lt;/wps:bodyPr&gt;&lt;/wps:wsp&gt;&lt;/a:graphicData&gt;&lt;/a:graphic&gt;&lt;wp14:sizeRelH relativeFrom="page"&gt;&lt;wp14:pctWidth&gt;0&lt;/wp14:pctWidth&gt;&lt;/wp14:sizeRelH&gt;&lt;wp14:sizeRelV relativeFrom="page"&gt;&lt;wp14:pctHeight&gt;0&lt;/wp14:pctHeight&gt;&lt;/wp14:sizeRelV&gt;&lt;/wp:anchor&gt;&lt;/w:drawing&gt;&lt;/mc:Choice&gt;&lt;mc:Fallback&gt;&lt;w:pict&gt;&lt;v:shape id="Полилиния 2" o:spid="_x0000_s1026" style="position:absolute;margin-left:340.9pt;margin-top:9.15pt;width:17pt;height:17pt;flip:x;z-index:251659264;visibility:visible;mso-wrap-style:square;mso-width-percent:0;mso-height-percent:0;mso-wrap-distance-left:9pt;mso-wrap-distance-top:0;mso-wrap-distance-right:9pt;mso-wrap-distance-bottom:0;mso-position-horizontal:absolute;mso-position-horizontal-relative:text;mso-position-vertical:absolute;mso-position-vertical-relative:text;mso-width-percent:0;mso-height-percent:0;mso-width-relative:page;mso-height-relative:page;v-text-anchor:top" coordsize="21600,21600" o:gfxdata="UEsDBBQABgAIAAAAIQC2gziS/gAAAOEBAAATAAAAW0NvbnRlbnRfVHlwZXNdLnhtbJSRQU7DMBBF&amp;#xA;90jcwfIWJU67QAgl6YK0S0CoHGBkTxKLZGx5TGhvj5O2G0SRWNoz/78nu9wcxkFMGNg6quQqL6RA&amp;#xA;0s5Y6ir5vt9lD1JwBDIwOMJKHpHlpr69KfdHjyxSmriSfYz+USnWPY7AufNIadK6MEJMx9ApD/oD&amp;#xA;OlTrorhX2lFEilmcO2RdNtjC5xDF9pCuTyYBB5bi6bQ4syoJ3g9WQ0ymaiLzg5KdCXlKLjvcW893&amp;#xA;SUOqXwnz5DrgnHtJTxOsQfEKIT7DmDSUCaxw7Rqn8787ZsmRM9e2VmPeBN4uqYvTtW7jvijg9N/y&amp;#xA;JsXecLq0q+WD6m8AAAD//wMAUEsDBBQABgAIAAAAIQA4/SH/1gAAAJQBAAALAAAAX3JlbHMvLnJl&amp;#xA;bHOkkMFqwzAMhu+DvYPRfXGawxijTi+j0GvpHsDYimMaW0Yy2fr2M4PBMnrbUb/Q94l/f/hMi1qR&amp;#xA;JVI2sOt6UJgd+ZiDgffL8ekFlFSbvV0oo4EbChzGx4f9GRdb25HMsYhqlCwG5lrLq9biZkxWOiqY&amp;#xA;22YiTra2kYMu1l1tQD30/bPm3wwYN0x18gb45AdQl1tp5j/sFB2T0FQ7R0nTNEV3j6o9feQzro1i&amp;#xA;OWA14Fm+Q8a1a8+Bvu/d/dMb2JY5uiPbhG/ktn4cqGU/er3pcvwCAAD//wMAUEsDBBQABgAIAAAA&amp;#xA;IQCZTmpCdQQAAPILAAAOAAAAZHJzL2Uyb0RvYy54bWysVm2O40QQ/Y/EHVr+CdqJ7cROHE1mtcwy&amp;#xA;AWmBlTYcoOOP2MJ2m25nktlLcASusRKCM4Qb8arb7TiZZFghRhqn7X5+VfWquly3r/dVyR5TqQpR&amp;#xA;LxzvxnVYWsciKerNwvl59fBq5jDV8jrhpajThfOUKuf13Zdf3O6aeeqLXJRJKhlIajXfNQsnb9tm&amp;#xA;PhqpOE8rrm5Ek9bYzISseItbuRklku/AXpUj33XD0U7IpJEiTpXC07dm07nT/FmWxu1PWabSlpUL&amp;#xA;B761+ir1dU3X0d0tn28kb/Ii7tzg/8GLihc1jPZUb3nL2VYWz6iqIpZCiay9iUU1EllWxKmOAdF4&amp;#xA;7lk0H3LepDoWiKOaXib1/9HGPz6+l6xIFo7vsJpXSNHh98Nfhz8On/T/n4dPf//GfNJp16g54B+a&amp;#xA;95IiVc07Ef+iWC3uc15v0jeqgdqoAfDYR1KKXZ7yBA57RDE64aAbBTa23v0gEljm21ZoFfeZrFhW&amp;#xA;Fs139CJZg1Jsr9P21Kct3bcsxkPfCyIXyY2x1a3JFp8TDb0cb1W7TIVe88d3qjVZT7DSOUu6yJcg&amp;#xA;yaoSBfD1K+YFnh8yl9ka6UEIsAf5kedfwkDMHuPBpxlAhO3qrecaD3BLYroEmljQVyO2HLOxPw1n&amp;#xA;uLpBdE4XDJET5pnEoSp7g6FFIELfC13EZyI9p5paIBkNtV8sdKfPTOJ895Eup1a1M7ZVLyzYjLA7&amp;#xA;Y/4c2IsLoMvyy6Be3X9j6+UloE7DFcahxGN/PGVX3BsKbOS7QtjrDMsGeIVxqDPpey3mXmcKZRpG&amp;#xA;k6nvIiH4Y2EQjMNzISObF+CDWTTzJy/CvWGGPgd/mqgXHEHRdxWikzDxr4rrDdO19K4p4Q2TtZxd&amp;#xA;S5U3zBXO1iBRaA0be/h5bvtBvK+7hoAVQ0tbOKuZbj6NUNR8qIrRYlamlaGt7GvdXXp0dIJG3IQe&amp;#xA;U2Zg8RkaktPrlhxRETy4CjeN0MJRYASfDuHGSheERDemr96KEoC+vCJ58eVbkX749q0gkO6DDW9J&amp;#xA;A+0LlmxHXRQJdVhuV7RXicd0JTSqJTU6DJywbQHmj6CyHoL1mdce63YKpN23v40mPeJsI7wO9VFK&amp;#xA;mvICNN6ui/ib9OPQhyAIjcYWD+21UZPWqRt07Xn4VHcNq/EJ6anjhsNoYvJt9+2vYQ0n084JLfFn&amp;#xA;QYc+WLZLAfbcnhsE3WfLWI28MfoBUhX5k65TmA2vF9HuUA29EOcxQYMXrFP2t+OmD6i2ejGAUqjU&amp;#xA;hE8FqI9IX4naieM3W4mySB6KsqTqU3Kzvi8le+Qo7gf91+XnBFbWVMhR4Af6lJ3snVBQC0WxG1dO&amp;#xA;YFXRYjYti2rhzHoQn9NA822d4AU+b3lRmrWu027CoaHGzEtrkTxhwJHCDJ4YlLHIhfzosB2GzoWj&amp;#xA;ft1ymTqs/L7GkBR5kwkqqdU3kwAtHkd2uLMe7vA6BtXCaR10K1ret7jDK9tGFptcz2LkZC3eYLDK&amp;#xA;Chp79ARmvOpuMFhq8bshmCbX4b1GHUf1u38AAAD//wMAUEsDBBQABgAIAAAAIQCJoqor3wAAAAkB&amp;#xA;AAAPAAAAZHJzL2Rvd25yZXYueG1sTI/BTsMwEETvSPyDtUjcqJOWlhDiVBUiFRJcKCCubrwkofY6&amp;#xA;it0m/D3LCY6zM5p5W6wnZ8UJh9B5UpDOEhBItTcdNQreXqurDESImoy2nlDBNwZYl+dnhc6NH+kF&amp;#xA;T7vYCC6hkGsFbYx9LmWoW3Q6zHyPxN6nH5yOLIdGmkGPXO6snCfJSjrdES+0usf7FuvD7ugUbJ9u&amp;#xA;r7df1eH9efShevQf9mFTW6UuL6bNHYiIU/wLwy8+o0PJTHt/JBOEVbDKUkaPbGQLEBy4SZd82CtY&amp;#xA;zhcgy0L+/6D8AQAA//8DAFBLAQItABQABgAIAAAAIQC2gziS/gAAAOEBAAATAAAAAAAAAAAAAAAA&amp;#xA;AAAAAABbQ29udGVudF9UeXBlc10ueG1sUEsBAi0AFAAGAAgAAAAhADj9If/WAAAAlAEAAAsAAAAA&amp;#xA;AAAAAAAAAAAALwEAAF9yZWxzLy5yZWxzUEsBAi0AFAAGAAgAAAAhAJlOakJ1BAAA8gsAAA4AAAAA&amp;#xA;AAAAAAAAAAAALgIAAGRycy9lMm9Eb2MueG1sUEsBAi0AFAAGAAgAAAAhAImiqivfAAAACQEAAA8A&amp;#xA;AAAAAAAAAAAAAAAAzwYAAGRycy9kb3ducmV2LnhtbFBLBQYAAAAABAAEAPMAAADbBwAAAAA=&amp;#xA;" o:allowincell="f" path="m21600,6079l15126,r,2912l12427,2912c5564,2912,,7052,,12158r,9442l6474,21600r,-9442c6474,10550,9139,9246,12427,9246r2699,l15126,12158,21600,6079xe"&gt;&lt;v:stroke joinstyle="miter"/&gt;&lt;v:path o:connecttype="custom" o:connectlocs="151190,0;151190,121524;32355,215900;215900,60762" o:connectangles="270,90,90,0" textboxrect="12427,2912,18227,9246"/&gt;&lt;o:lock v:ext="edit" aspectratio="t"/&gt;&lt;/v:shape&gt;&lt;/w:pict&gt;&lt;/mc:Fallback&gt;&lt;/mc:AlternateContent&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;СМОТРИТЕ ОБОРОТ БЛАНКА&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;ОПЕРАТОР ИМЕЕТ ПРАВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обрабатывать персональные данные посредством внесения их в электронную базу данных, включения в списки (реестры) и отчетные формы, предусмотренные документами, регламентирующими предоставление отчетных данных (документов) по договору ОМС/ДМС, договору ока&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;зания платных медицинских услуг; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;осуществлять обмен (прием и передачу) персональными данными со страховой медицинской организацией, организацией - заказчиком медицинских услуг во исполнение своих обязательств по договору ДМС, договору оказания платных меди&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;цинских услуг с использованием машинных носителей информации, по каналам связи и (или) документы на бумажных носителях, с соблюдением мер, обеспечивающих их защиту от несанкционированного доступа, без специального уведомления меня об этом, при условии, что&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; их&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt; прием и обработка будут осуществляться лицом,  обязанным сохранять профессиональную (служебную) тайну.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Срок хранения персональных данных&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; соответствует сроку хранения первичных медицинских документов (медицинской карты) и &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;составляет двадцать пять лет &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;для стационара, пять лет – для поликлиники&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Передача персональных данных иным лицам или иное их разглашение может осуществляться &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;только с моего письменного согласия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НАСТОЯЩЕЕ СОГЛАСИЕ действует  бессрочно, и может быть отозвано мною путем направления в а&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;дрес Оператора соответствующего письменного документа (по почте заказным письмом с уведомление&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;м о вручении) либо путем вручения лично под расписку представителю Оператора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CE4ADC" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Подпись субъекта персональных данных       ____________________________________    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;        &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (или его законного представителя)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;____________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;      (Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сведения в электронную базу данных внесены:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="right"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Оператор: __________________________________          &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;           ______________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00970840" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="1416" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B1288F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DA63DE" w:rsidRPr="00B1288F" w:rsidRDefault="009954EA" w:rsidP="00B1288F"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00DA63DE" w:rsidRPr="00B1288F" w:rsidSect="00B1288F"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AgreementMedicalIntervention</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Согласие на медицинское вмешательство</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
-&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ИНФОРМИРОВАННОЕ ДОБРОВОЛЬНОЕ СОГЛАСИЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НА МЕДИЦИНСКОЕ ВМЕШАТЕЛЬСТВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="10"/&gt;&lt;w:szCs w:val="10"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00830DEA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Я, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нижеподписавшийся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;аяся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="009E76EC"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;,&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обратившись за получением медицинских услуг в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;обособленное структурное подразделение – &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;NIKIName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;,   в соответствии с &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Приказом МЗ СР РФ от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;23.04.2012 г. N 390-н&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; даю согласие на проведение&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; пациенту &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                  &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;при необходимости следующих вмешательст&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;в: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. Опрос, в том числе выявление жалоб, сбор анамнеза. 2. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Осмотр, в том числе пальпация, перкуссия, аускультация, риноскопия, фарингоскопия, непрямая ларингоскопия, вагинальное исследование (для женщин). 3.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Антропометрические исследования; 4. Термометрия; 5. Тонометрия. 6. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Неинвазивные&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования органа зрения &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;и зрительных функций. 7. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Неинвазивные&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования органа слуха и слуховых функций. 8. Исследование функций нервной системы (чувствительной и двигательной сферы). 9. Лабораторные методы обследования, в том числе клинические, биохимические, бактериологическ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ие, вирусологические, иммунологические (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;со&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; взятием крови из пальца и вены). 10. Функциональные методы обследования, в том числе электрокардиография (ЭКГ), суточное &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мониторирование&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; артериального давления, суточное &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мониторирование&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; электрокардиограммы, спирог&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;рафия, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пневмотахометрия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пикфлуометрия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;рэоэнцефалография&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, электроэнцефалография. 11. Рентгенологические методы обследования, в том числе флюорография (для лиц старше 15 лет) и рентгенография, ультразвуковые исследования, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;допплерографические&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; исследования. &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;12. Введение лекарственных препаратов по назначению врача, в том числе внутримышечно, внутривенно, подкожно, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;внутрикожно&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;. 13. Медицинский массаж, ЛФК.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я понимаю&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, что во время вмешательства или после него могут появиться непредвиденные ранее неблагоприятные&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обстоятельства, а также могут возникнуть осложнения. При этом медицинские работники делают все возможное для предотвращения возможных осложнений в соответствии с действующими порядками и стандартами  оказания медицинской помощи. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я предупрежден&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, что невып&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;олнение в полном объёме всех рекомендаций медицинского работника может быть причиной осложнений и неблагоприятных последствий медицинского вмешательства.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="10"/&gt;&lt;w:szCs w:val="10"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ПОДПИСЬ: _________________________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt; __________________________________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRDefault="009E76EC" w:rsidP="00803FC9"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(пациента старше 15 лет, матери / отца / официального опекуна)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00803FC9" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00803FC9"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="264" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00B51C43" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC" w:rsidP="00B51C43"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПОДПИСЬ ВРАЧА: ____________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;                __________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00803FC9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DA63DE" w:rsidRPr="00803FC9" w:rsidRDefault="009E76EC"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00DA63DE" w:rsidRPr="00803FC9" w:rsidSect="00803FC9"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ДОБРОВОЛЬНОЕ ИНФОРМИРОВАННОЕ СОГЛАСИЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на обработку персональных данных&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Я, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нижеподписавшийся&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ClientIdentityDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;RelativeTypeName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientFullName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00A64992" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Документ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;удостоверяющий&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;личность&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientIdentityDocument&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="00A64992" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Адрес пациента: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;PatientAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00A64992"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;В соответствии с требованиями&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; статьи 9 Федерального закона "О персональных данных" от 27.07.2006 N 152-ФЗ, статьи 13 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Федерального закона от 21.11.2011 N 323-ФЗ "Об основах охраны здоровья граждан в РФ"&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПОДТВЕРЖДАЮ СВОЕ СОГЛАСИЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; на обработку &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:iCs/&gt;&lt;w:noProof/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgAddress&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;) (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;далее - Оператор&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;моих персональных данных, персональных данных представляемого мной (сына, дочери, опекаемого) ____________________________________________________________________________________(Ф.И.О.),&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;включающих: фамилию, имя, отчество, пол, дату рождения, адрес места &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;жительства, контактные телефоны, реквизиты паспорта (документа удостоверения личности, в том числе свидетельства о рождении), реквизиты полиса ОМС/ДМС, страховой номер индивидуального лицевого счета в Пенсионном фонде России (СНИЛС), место работы, учебы, д&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;анные о состоянии здоровья, заболеваниях, случаях обращения за медицинской помощью и другую информацию - в медико-профилактических целях, в целях установления медицинского&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; диагноза и оказания медицинских услуг по договору, осуществление иных, связанных с э&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;тим мероприятий, а также в целях организации внутреннего учета Оператора, при условии сохранения врачебной тайны (или – при условии, что эта обработка осуществляется лицом, уполномоченным Оператором и обязанным сохранять &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;профес&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.т&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;айну&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;). &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;В процессе оказания&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Оператором &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;мне/представляемому мной ребенку в возрасте до 15 лет&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинских услуг &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПРЕДОСТАВЛЯЮ ПРАВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинским работникам (врачам, среднему медицинскому персоналу) передавать мои персональные данные/персональные данные представляемого мной ребенка в&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; возрасте до 15 лет, в том числе составляющие врачебную тайну, другим должностным лицам Оператора в интересах обследования, лечения и внутреннего учета Оператора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я СОГЛАСЕН (-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НА&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; осмотр другими медицинскими работниками и  студентами медицинских вузов/ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Arial" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="hi-IN" w:bidi="hi-IN"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;колледжей исключительно в медицинских, научных или обучающих целях с учетом сохранения врачебной тайны.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ПРЕДОСТАВЛЯЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ОПЕРАТОРУ ПРАВО ОСУЩЕСТВЛЯТЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; все действия (операции) с  персональными данными, включая сбор, систематизацию, накопление, хранение, обновление, изменение, использование, передачу (в страховую медицинскую организацию, организацию - заказчика медицинских услуг в рамках заключенных догов&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;оров), обезличивание, блокирование, уничтожение.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ОПЕРАТОР ВПРАВЕ ОСУЩЕСТВЛЯТЬ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; следующие способы обработки персональных данных: на бумажных носителях, в информационных системах персональных данных с использованием и без использования средств автоматизации, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;а также смешанным способом.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Я ДАЮ СОГЛАСИЕ / НЕ ДАЮ СОГЛАСИЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нужное подчеркнуть, ненужное зачеркнуть&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператору на использование персональных данных в целях информирования меня с помощью средств связи путем пересылки мне SMS-сообщений: напоминание о запис&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;и на прием к специалисту или исследование (на указанный мной номер мобильного телефона), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на пересылку информации о состоянии здоровья моего ребенка (результаты дополнительных методов обследования и др.) через незащищенные каналы связи&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (электронная почта), &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;для чего &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;собственноручно пишу адрес электронной почты и телефон&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, на который разрешаю высылать данные о состоянии здоровья и иные сведения: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;E&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;mail&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; __________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Телефон:___________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подпись субъекта персональных данных   ________________             ____________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(или его законного представителя)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сведения в электронную базу данных внесены:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператор: __________________________________                        ______________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="708" w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:br w:type="page"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;ОПЕРАТОР ИМЕЕТ ПРАВО&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; обрабатывать персональные данные посредством &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;внесения их в электронную базу данных, включения в списки (реестры) и отчетные формы, предусмотренные документами, регламентирующими предоставление отчетных данных (документов) по договору ОМС/ДМС, договору оказания платных медицинских услуг; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;осуществлять &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;обмен (прием и передачу) персональными данными со страховой медицинской организацией, организацией - заказчиком медицинских услуг во исполнение своих обязательств по договору ДМС, договору оказания платных медицинских услуг с использованием машинных носите&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;лей информации, по каналам связи и (или) документы на бумажных носителях, с соблюдением мер, обеспечивающих их защиту от несанкционированного доступа, без специального уведомления меня об этом, при условии, что их&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt; прием и обработка будут осуществляться лиц&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ом,  обязанным сохранять профессиональную (служебную) тайну.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Срок хранения персональных данных&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; соответствует сроку хранения первичных медицинских документов (медицинской карты) и &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;составляет двадцать пять лет для стационара, пять лет – для поликлиники&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Передача персональных данных иным лицам или иное их разглашение может осуществляться &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;только с моего письменного согласия&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НАСТОЯЩЕЕ СОГЛАСИЕ действует  бессрочно, и может быть отозвано мною путем направления в адрес Оператора соответствующего письменного д&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;окумента (по почте заказным письмом с уведомление&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;м о вручении) либо путем вручения лично под расписку представителю Оператора.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подпись субъекта персональных данных   ________________       ________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(или его законного представителя)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сведения в электронную базу данных внесены:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:eastAsia="ar-SA"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Оператор: _______________________________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;           ______________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00CB2697" w:rsidRPr="0018500E" w:rsidRDefault="00A64992" w:rsidP="00285CD3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:ind w:left="708" w:firstLine="708"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t xml:space="preserve"&gt;            &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0018500E"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00CB2697" w:rsidRPr="0018500E"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="1134" w:right="850" w:bottom="1134" w:left="1701" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>ProvidingConfidentialInformation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Согласие о порядке предоставления конфиденциальной информации</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
-&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ДОБРОВОЛЬНОЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ИНФОРМИРОВАННОЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; СОГЛАСИЕ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;О ПОРЯДКЕ ПРЕДОСТАВЛЕНИЯ КОНФИДЕНЦИАЛЬНОЙ ИНФОРМАЦИИ&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Я &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;РАЗРЕШАЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; / НЕ РАЗРЕШАЮ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ненужное зачеркнуть&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в соответствии с пунктом 5 части 3 статьи 19 Федерального зако&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;на от 21.11.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;2011 г. N 323-ФЗ "Об основах охраны здоровья граждан в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;РФ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;" предоставлять сведения о фактах моего обращения за медицинской помощью и состоянии здоровья, диагнозе, в т. ч. через регистратуру, а также в случаях неблагоприятного прогноза развития моего заболев&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ания &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;следующим лицам&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Ф.И.О. полностью,  контактный телефон) &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:br/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:br/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О. полностью,  контактный телефон)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______________________      ______________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;               (подпись)                             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;        &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Ф.И.О. пациента &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;старше&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; 15 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;лет или законного представителя пациента младше 15 лет)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;CurrentDate&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:autoSpaceDE w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="007D5E80" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F" w:rsidP="007D5E80"&gt;&lt;w:pPr&gt;&lt;w:snapToGrid w:val="0"/&gt;&lt;w:spacing w:after="0" w:line="240" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Оператор:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;____ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(подпись)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;             &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B9194F"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00DA63DE" w:rsidRPr="00B9194F" w:rsidRDefault="00B9194F"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00DA63DE" w:rsidRPr="00B9194F" w:rsidSect="00325796"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="851" w:right="737" w:bottom="567" w:left="1361" w:header="709" w:footer="709" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+    <x:t>SelectionHMHCommissionJournal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Журнал комиссии по отбору пациентов на ВМП</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00E8624D" w:rsidRPr="009E3920" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009E3920"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00E8624D" w:rsidRPr="009E3920" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00E8624D" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="009E3920"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="5000" w:type="pct"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tblBorders&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="0000" w:firstRow="0" w:lastRow="0" w:firstColumn="0" w:lastColumn="0" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="481"/&gt;&lt;w:gridCol w:w="725"/&gt;&lt;w:gridCol w:w="1007"/&gt;&lt;w:gridCol w:w="684"/&gt;&lt;w:gridCol w:w="688"/&gt;&lt;w:gridCol w:w="818"/&gt;&lt;w:gridCol w:w="860"/&gt;&lt;w:gridCol w:w="581"/&gt;&lt;w:gridCol w:w="724"/&gt;&lt;w:gridCol w:w="1007"/&gt;&lt;w:gridCol w:w="749"/&gt;&lt;w:gridCol w:w="678"/&gt;&lt;w:gridCol w:w="707"/&gt;&lt;w:gridCol w:w="478"/&gt;&lt;w:gridCol w:w="608"/&gt;&lt;w:gridCol w:w="823"/&gt;&lt;w:gridCol w:w="1106"/&gt;&lt;w:gridCol w:w="1094"/&gt;&lt;w:gridCol w:w="791"/&gt;&lt;w:gridCol w:w="868"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidTr="004058A1"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Число, месяц, год &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="272" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="001F16E9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;протокола&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата принятия документов к рассмотрению&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="226" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Фамилия, имя, отчество пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="227" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата рождения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="258" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Адрес, указанный в документах&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="268" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="00CB3600"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Контактный телефон&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; п&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="202" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Диагноз&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="236" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код основного диагноза по МКБ-10&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Случай обращения, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;который стал поводом к рассмотрению документов на Комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="249" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="006421FB"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата принятия решения &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="006421FB"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;к&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;омиссией&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="225" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Решение комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="232" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Состав Комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№ талона ВМП&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="208" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="006421FB"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код вида ВМП&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="006421FB"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; и&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ли профиль СМП&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="259" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="006421FB"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата отправки документов&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="006421FB"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;заявителю&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="327" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="006421FB"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="006421FB"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;планируемой госпитализации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="324" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Отделение куда планиру&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ется госпитализация&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="252" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="006421FB"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата выписки  из стационара&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidR="006421FB"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Центра&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="270" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Примечание&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidTr="004058A1"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="272" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="226" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="227" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;5&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="258" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="268" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="202" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="236" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="249" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="225" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;12&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="232" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;13&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;14&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="208" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;15&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="259" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;16&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="327" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;17&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="324" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;18&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="252" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;19&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="270" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00CA6D40"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;20&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidTr="004058A1"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00E8624D" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="272" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="226" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="227" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="258" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="268" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="202" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="236" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="303" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="249" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="225" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="232" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="178" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="208" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="259" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="327" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="324" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="252" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="270" w:type="pct"/&gt;&lt;w:tcBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tcBorders&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="00CA6D40" w:rsidRDefault="00CB3600" w:rsidP="004058A1"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="009E3920" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="009E3920" w:rsidRPr="009E3920" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00E8624D" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="006E3075" w:rsidRDefault="00CB3600" w:rsidP="00E8624D"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="006E3075" w:rsidSect="006E3075"&gt;&lt;w:pgSz w:w="16838" w:h="11906" w:orient="landscape"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KILIJournal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Журнал КИЛИ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00B96DB2" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00B96DB2"&gt;&lt;w:pPr&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="0" w:type="auto"/&gt;&lt;w:tblInd w:w="10" w:type="dxa"/&gt;&lt;w:tblBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideH w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideV w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tblBorders&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="1211"/&gt;&lt;w:gridCol w:w="1241"/&gt;&lt;w:gridCol w:w="1239"/&gt;&lt;w:gridCol w:w="1241"/&gt;&lt;w:gridCol w:w="1265"/&gt;&lt;w:gridCol w:w="1282"/&gt;&lt;w:gridCol w:w="1223"/&gt;&lt;w:gridCol w:w="1263"/&gt;&lt;w:gridCol w:w="1668"/&gt;&lt;w:gridCol w:w="1264"/&gt;&lt;w:gridCol w:w="1258"/&gt;&lt;w:gridCol w:w="1253"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="00506B95" w:rsidTr="00EB162B"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;N&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п/п&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Д&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ата заседа&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ния&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Состав&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;к&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;омиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Ф.И.О. умершего больного, дата рождения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№ меди&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;цинской&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; карты&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, протокола вскрытия)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата госпитали&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;зации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата смерти&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Диагноз клинический&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Диагноз &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;атологоанатоми&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ческий (судебно-медицинский)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Расхождение &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;диагнозов&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Наличие ятрогенных ослож&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нений&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Подписи участ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ников комиссии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00506B95" w:rsidTr="00EB162B"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;5&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00506B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;12&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00506B95" w:rsidTr="00EB162B"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1300" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1301" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1302" w:type="dxa"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00506B95" w:rsidRPr="00506B95" w:rsidRDefault="00EB162B" w:rsidP="00EB162B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:lang w:val="en-US" w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;tblval&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="00B96DB2" w:rsidRDefault="00EB162B" w:rsidP="00B96DB2"&gt;&lt;w:pPr&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Calibri" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:eastAsia="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="00B96DB2" w:rsidRDefault="00EB162B" w:rsidP="00B96DB2"&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="00B96DB2" w:rsidSect="006E3075"&gt;&lt;w:pgSz w:w="16838" w:h="11906" w:orient="landscape"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ReferralToHospitalisationCommission</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Направление на комисию по отбору пациентов на госпитализацию</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент (ФИО; возраст):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00F974CA" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00F974CA" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Диагноз:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код МКБ-10:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00F974CA" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Планируется  госпитализация  на ________________________(число; месяц; год):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;в соответствии с пп.14.15,16 приказа № 406н от 26.04.2012г. «Об утверждении порядка выбора  гражданином медицинской&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; организации при оказании ему медицинской помощи в рамках программы государственных гарантий  бесплатного оказания  гражданам медицинской помощи», пациент информирован о том, что срок ожидания специализированной медицинской помощи превышает срок ожидания м&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;едицинской помощи, установленный территориальной программой  и что он   имеет возможность  получить необходимую помощь в другой&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинской организации. &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент выбрал госпитализацию в Институт.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Профиль медицинской помощи  и отделение, куда планируется г&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;оспитализация:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код вида ВМП (в случае планирования госпитализации по ВМП):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Лечащий врач:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заведующий отделением:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00C56C6C" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00F974CA"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Печать:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="00F974CA" w:rsidRDefault="00F974CA" w:rsidP="00F974CA"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:sz w:val="20"/&gt;&lt;w:szCs w:val="20"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="00F974CA" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CommonCommissionProtocol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Общий протокол комиссии</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="001B0874" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:sz w:val="12"/&gt;&lt;w:szCs w:val="12"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:color w:val="000000"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="002A7F05" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00D274C6" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ПРОТОКОЛ &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; _______&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;          &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007E4400"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«_____»&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D274C6"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;201___ г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="002A7F05" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="003F2B9A" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:caps/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="003F2B9A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:caps/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Комиссия в составе: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Председатель: _____________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00FC20C9" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заместитель председателя: ____________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Секретарь комиссии: _________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="000C2257" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Присутствовали &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Члены комиссии:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(должность, Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(должность, Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(должность, Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(должность, Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="00AD5078"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AD5078"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="16"/&gt;&lt;w:szCs w:val="16"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(должность, Ф.И.О.)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="00AD5078" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00AA6624" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00AA6624"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Рассмотрела медицинские документы и/или исто&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;рию болезн&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;и № _______________ &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00AA6624" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00AA6624"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00AA6624"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;_______________, ______________ года рождения, &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="0052088B" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0052088B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ДИАГНОЗ:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0052088B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0052088B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;______________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="003F2B9A" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="003F2B9A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="003F2B9A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________________.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="0052088B" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="12"/&gt;&lt;w:szCs w:val="12"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="007D4DE9" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="0052088B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:caps/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заключение комиссии:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="0052088B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;В соответствии с Федеральным законом &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:color w:val="000000"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;от 12&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:color w:val="000000"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.04.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:color w:val="000000"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2010 г. N 61-&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ФЗ "Об обращении лекарственных средств", Приказом МЗ и СР России  №502н от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;05.05.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2012 г&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; «Об утверждении порядка создания и деятельности врачебной&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; комиссии медицинской организации»,  Приказом &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Минздрава РФ № 1175-н от 20.12.2012&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;г. «Об утверждении порядка назначения и выписывания лекарственных препаратов» (в ред. Приказа МЗ РФ от &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;02.12.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2013 г.&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;N 886н)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ребенку &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;по&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; медицинским  показаниям назначено 5 и более препаратов&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D4DE9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:i/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="007D36C4" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="007D36C4" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_______________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="008B6C3C" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="FF0000"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008B6C3C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:color w:val="FF0000"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (перечислить ЛС и написать обоснование назначения 5 и более препаратов)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00111459" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="10"/&gt;&lt;w:szCs w:val="10"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="007D36C4" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="007D36C4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;НАЗНАЧЕНИЯ СОГЛАСОВАНЫ.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="004E6603" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="12"/&gt;&lt;w:szCs w:val="12"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="23"/&gt;&lt;w:szCs w:val="23"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00AD5078" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Председатель:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:bCs/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="0014106F" w:rsidRPr="00FC20C9" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:ind w:left="-142"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Секретарь: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00FC20C9"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="0014106F" w:rsidRDefault="007D4DE9" w:rsidP="0038565A"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="0014106F" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CommonConsiliumProtocol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Общий протокол консилиума врачей</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00CB40B2" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00732B10"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EA0453"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00CB40B2" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="28"/&gt;&lt;w:szCs w:val="28"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="003B316C" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;КОНСИЛИУМ ВРАЧЕЙ В СОСТАВЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="003B316C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="003B316C" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Лечащий врач &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;            _____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:ind w:left="2832" w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;(Ф.И.О., специализация, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;квалификация)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заведующий отделением __________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:ind w:left="2832" w:firstLine="708"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О., специализация, квалификация)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Участники консилиума:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; __________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                                   &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00B34B15"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О., должность, специализация, квалификация)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заведующий/сотрудник научного отдела:___________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;__________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                                                  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О., должность, специализация, квалификация)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата, время и место проведения консилиума&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00DE2768" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Данные о пациенте&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (Ф.И.О., дата рождения, адре&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;с места жительства&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;):_______________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Данные о состоянии &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; жалобы, краткий анамнез, результаты осмотра, данные лабораторных и инструментальных обследований): &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="28"/&gt;&lt;w:szCs w:val="28"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заключение &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00DE2768"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:sz w:val="28"/&gt;&lt;w:szCs w:val="28"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;консилиума&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____________________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;С содержанием заключения &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ознакомлен&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (в случае присутствия пациента на консилиуме):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_________________________________________________________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;(Ф.И.О. и подпись пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; и /&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; или его законного представителя)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="003B316C" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00774081"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ПОДПИСИ УЧАСТНИКОВ КОНСИЛИУМА&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="003B316C"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________________________ (расшифровка подписи)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;________________________________ (расшифровка подписи)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00EE03E3" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;_____________________________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00EE03E3"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___ (расшифровка подписи)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E3075" w:rsidRPr="00732B10" w:rsidRDefault="00CB40B2" w:rsidP="00CB40B2"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="006E3075" w:rsidRPr="00732B10" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NoticeSideEffects</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Извещение о побочном действии ЛС</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00732B10"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00732B10" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00084B95" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00084B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="5000" w:type="pct"/&gt;&lt;w:tblInd w:w="28" w:type="dxa"/&gt;&lt;w:tblBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideH w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideV w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tblBorders&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="01E0" w:firstRow="1" w:lastRow="1" w:firstColumn="1" w:lastColumn="1" w:noHBand="0" w:noVBand="0"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="1487"/&gt;&lt;w:gridCol w:w="983"/&gt;&lt;w:gridCol w:w="259"/&gt;&lt;w:gridCol w:w="274"/&gt;&lt;w:gridCol w:w="467"/&gt;&lt;w:gridCol w:w="1155"/&gt;&lt;w:gridCol w:w="495"/&gt;&lt;w:gridCol w:w="158"/&gt;&lt;w:gridCol w:w="63"/&gt;&lt;w:gridCol w:w="179"/&gt;&lt;w:gridCol w:w="888"/&gt;&lt;w:gridCol w:w="133"/&gt;&lt;w:gridCol w:w="1000"/&gt;&lt;w:gridCol w:w="141"/&gt;&lt;w:gridCol w:w="709"/&gt;&lt;w:gridCol w:w="16"/&gt;&lt;w:gridCol w:w="125"/&gt;&lt;w:gridCol w:w="1990"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="2008"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2617" w:type="pct"/&gt;&lt;w:gridSpan w:val="10"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ВРАЧ или другое лицо, сообщающее о НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ФИО:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Должность  и место работы:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Адрес учреждения:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Телефон:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата получения информации:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2383" w:type="pct"/&gt;&lt;w:gridSpan w:val="8"/&gt;&lt;w:vMerge w:val="restart"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ИНФОРМАЦИЯ О ПАЦИЕНТЕ&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Инициалы:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№ амбулаторной карты или истории болезни __________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Пол:   &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; М                      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; Ж&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Возраст: _________       Вес (&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;кг&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;): __________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Беременность  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;   Срок беременности _____недель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Нарушение функции печени  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; да  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нет&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  не известно&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Нарушение функции почек     &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; да  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;нет&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  не известно&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Аллергия (указать на ч&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;то):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="534"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2617" w:type="pct"/&gt;&lt;w:gridSpan w:val="10"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Лечение: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; амбулаторное    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; стационарное   &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; самолечение&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Сообщение: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; первичное &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                      &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; повторное (дата первичного     _________&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  )&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2383" w:type="pct"/&gt;&lt;w:gridSpan w:val="8"/&gt;&lt;w:vMerge/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="363"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ЛЕКАРСТВЕННОЕ СРЕДСТВО (ЛС) №1, предположительно вызвавшее НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="444"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1415" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Международное непатентованное &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;название (МНН)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1689" w:type="pct"/&gt;&lt;w:gridSpan w:val="8"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="544" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Торговое название &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1352" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="301"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="692" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Производитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Страна&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="882" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Номер серии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1014" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="474"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Показание к назначению&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Путь введения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Разовая/Суточная доза&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата начала терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="882" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата окончания терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1014" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Доза, вызвавшая НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="350"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="882" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1014" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="363"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;ЛЕКАРСТВЕННОЕ СРЕДСТВО (ЛС) №2, &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;предположительно вызвавшее НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="444"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1415" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Международное непатентованное название (МНН)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1689" w:type="pct"/&gt;&lt;w:gridSpan w:val="8"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="544" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Торговое название&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1352" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="301"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="692" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Производитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Страна&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Номер серии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="474"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Показание к назначению&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Путь введения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Разовая/Суточная доза&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата начала терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата окончания терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Доза, вызвавшая НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="350"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="363"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ЛЕКАРСТВЕННОЕ СРЕДСТВО (ЛС) №3, предположительно вызвавшее НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="444"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1415" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Международное непатентованное название (МНН)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1689" w:type="pct"/&gt;&lt;w:gridSpan w:val="8"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="544" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Торговое название&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1352" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="301"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="692" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Производитель&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Страна&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Номер серии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="474"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Показание к назначению&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Путь введения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Разовая/Суточная доза&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;начала терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата окончания терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Доза, вызвавшая НР&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="350"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1160" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="478" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="786" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="680" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="890" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1006" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="535"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ДРУГИЕ ЛЕКАРСТВЕННЫЕ СРЕДСТВА, принимаемые в течение последних 3 месяцев, включая ЛС принимаемые пациентом самостоятельно (по собственному решению)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00A4093A" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Укажите &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;«НЕТ»&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;, если &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00A4093A"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;других лекарств пациент не принимал&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:cantSplit/&gt;&lt;w:trHeight w:val="227"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1284" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;МНН&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1216" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ТН&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Путь введения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата начала терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="474" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата окончания терапии&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Показание&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:cantSplit/&gt;&lt;w:trHeight w:val="454"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1284" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1216" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="474" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:cantSplit/&gt;&lt;w:trHeight w:val="454"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1284" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1216" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="474" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:cantSplit/&gt;&lt;w:trHeight w:val="454"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1284" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1216" w:type="pct"/&gt;&lt;w:gridSpan w:val="5"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="3"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="540" w:type="pct"/&gt;&lt;w:gridSpan w:val="2"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="474" w:type="pct"/&gt;&lt;w:gridSpan w:val="4"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;/       /&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="2073"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="4054" w:type="pct"/&gt;&lt;w:gridSpan w:val="17"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:lastRenderedPageBreak/&gt;&lt;w:t&gt;Описание НР:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="946" w:type="pct"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата начала НР:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;___/_____/______&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата разрешения:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;____/___ /______&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="493"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сопровождалось ли отмена ЛС исчезновением НР?&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;     &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; да    &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;нет   &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  ЛС не отменялось&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  неприменимо&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="515"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Отмечено ли повторение НР после повторного назначения ЛС?&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; да &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;нет &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  ЛС повторно не назначалось&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F06F"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  неприменимо&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="726"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2188" w:type="pct"/&gt;&lt;w:gridSpan w:val="6"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Предпринятые меры:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  Без лечения                                                                           &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  Отмена &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;подозреваемого&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ЛС&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  Снижение дозы &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;подозреваемого&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; ЛС                                   &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2812" w:type="pct"/&gt;&lt;w:gridSpan w:val="12"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:numPr&gt;&lt;w:ilvl w:val="0"/&gt;&lt;w:numId w:val="1"/&gt;&lt;/w:numPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="clear" w:pos="720"/&gt;&lt;w:tab w:val="num" w:pos="252"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="0" w:firstLine="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Отмена сопутствующего лечения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:numPr&gt;&lt;w:ilvl w:val="0"/&gt;&lt;w:numId w:val="1"/&gt;&lt;/w:numPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="clear" w:pos="720"/&gt;&lt;w:tab w:val="num" w:pos="252"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:ind w:left="0" w:firstLine="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Лекарственная терапия                 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;                                       &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  Немедикаментозная терапия (в &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;т.ч&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;. хирургическое вмешательство) &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;  Другое,  указать ________________________________                                                                                                 &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;           &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="817"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="left" w:pos="4308"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Лекарственная терапия  НР (если понадобилась)&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;    &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="1393"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2531" w:type="pct"/&gt;&lt;w:gridSpan w:val="9"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Исход:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; выздоровление без последствий                                          &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="num" w:pos="252"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; улучшение состояния&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; состояние без изменений&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; выздоровление с последствиями (указать)_____________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2469" w:type="pct"/&gt;&lt;w:gridSpan w:val="9"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; смерть                                                                                    &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; не известно&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; не применимо&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="1220"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2531" w:type="pct"/&gt;&lt;w:gridSpan w:val="9"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Критерий серьезности (отметьте, если это подходит):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; смерть                                         &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="num" w:pos="252"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; угроза жизни&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; госпитализация &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;или ее продление&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="2469" w:type="pct"/&gt;&lt;w:gridSpan w:val="9"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; врожденные аномалии                                                                                    &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; инвалидность / нетрудоспособность&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:tabs&gt;&lt;w:tab w:val="left" w:pos="252"/&gt;&lt;/w:tabs&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:sym w:font="Wingdings" w:char="F0A8"/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00957D09"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="19"/&gt;&lt;w:szCs w:val="19"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; не применимо&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:trHeight w:val="3034"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="5000" w:type="pct"/&gt;&lt;w:gridSpan w:val="18"/&gt;&lt;w:tcMar&gt;&lt;w:top w:w="28" w:type="dxa"/&gt;&lt;w:left w:w="28" w:type="dxa"/&gt;&lt;w:bottom w:w="28" w:type="dxa"/&gt;&lt;w:right w:w="28" w:type="dxa"/&gt;&lt;/w:tcMar&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Значимая дополнительная информация&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Данные клинических, лабораторных, рентгенологических исследований и аутопсии, включая определение концентрации ЛС в крови/тканях, если таковые имеются и связаны с НР (пожалуйста, приведите даты). &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сопутствующие заболевания. Анамнестические данные, подозрев&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;аемые лекарственные взаимодействия.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00D03A76" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00D03A76"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:i/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Для врожденных аномалий указать все другие ЛС, принимаемые во время беременности, а также дату последней менструации. Пожалуйста, приложите дополнительные страницы, если это необходимо.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00957D09" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="283" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="18"/&gt;&lt;w:szCs w:val="18"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidRDefault="00D15F58" w:rsidP="00D15F58"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SanCurCard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Карта пациента при направлении на сан-кур</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00732B10"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00732B10" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00084B95" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00084B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:tbl&gt;&lt;w:tblPr&gt;&lt;w:tblW w:w="5000" w:type="pct"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:tblBorders&gt;&lt;w:top w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:left w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:bottom w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:right w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideH w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;w:insideV w:val="single" w:sz="4" w:space="0" w:color="auto"/&gt;&lt;/w:tblBorders&gt;&lt;w:tblCellMar&gt;&lt;w:left w:w="10" w:type="dxa"/&gt;&lt;w:right w:w="10" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;w:tblLook w:val="04A0" w:firstRow="1" w:lastRow="0" w:firstColumn="1" w:lastColumn="0" w:noHBand="0" w:noVBand="1"/&gt;&lt;/w:tblPr&gt;&lt;w:tblGrid&gt;&lt;w:gridCol w:w="835"/&gt;&lt;w:gridCol w:w="3322"/&gt;&lt;w:gridCol w:w="6329"/&gt;&lt;/w:tblGrid&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п\&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;п&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;П&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;араметры&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;w:vAlign w:val="center"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Сведения о пациенте&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;1&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Фамилия&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;2&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Имя&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;3&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Отчество&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;4.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Документ, удостоверяющий личность пациента&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код вида документа&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Серия документа&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Номер документа&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;5.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;СНИЛС&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;6.&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Страховой полис ОМС:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Наименование страховой &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;компании&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Серия полиса&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Номер полиса&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;7&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Адресная информация:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Почтовый индекс&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Субъект Российской Федерации&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Район&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Населенный пункт&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Улица&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дом&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Корпус&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Строение&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;квартира&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;8&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;П&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;ол&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;9&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата рождения&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;10&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Дата регистрации пациента в системе&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;w:tr w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidTr="006A6E60"&gt;&lt;w:tblPrEx&gt;&lt;w:tblCellMar&gt;&lt;w:top w:w="0" w:type="dxa"/&gt;&lt;w:bottom w:w="0" w:type="dxa"/&gt;&lt;/w:tblCellMar&gt;&lt;/w:tblPrEx&gt;&lt;w:trPr&gt;&lt;w:jc w:val="center"/&gt;&lt;/w:trPr&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="398" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;11&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="1584" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Социальная группа&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="008363E8"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; (дошкольник, школьник, студент)&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;w:tc&gt;&lt;w:tcPr&gt;&lt;w:tcW w:w="3018" w:type="pct"/&gt;&lt;w:shd w:val="clear" w:color="auto" w:fill="auto"/&gt;&lt;/w:tcPr&gt;&lt;w:p w:rsidR="006E4DFB" w:rsidRPr="008363E8" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;/w:tc&gt;&lt;/w:tr&gt;&lt;/w:tbl&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidRDefault="00890056" w:rsidP="00890056"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExcerptCommissionProtocol</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Выписка из протокола решения врачебной комиссии </x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00732B10"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;OrgName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00732B10" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00084B95" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00084B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;г. Москва &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:tab/&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;№ ____________&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Ф.И.О. пациента: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата рождения: &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Адрес&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Lucida Sans Unicode" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;регистрации по месту жительства (пребывания): &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Код диагноза по МКБ – 10: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Основной диагноз:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Номер талона (в случае высокотехнологичной медицинской помощи): &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Заключение Комиссии (направить на &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;дообследование&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;, оказать ВМП/ВМП в ОМС, отказать в ВМП, отказать в СМП, госпитализация для оказания&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;СМП): &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="gramStart"/&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код вида ВМП (в случае решения о показаниях к ВМП:&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="gramEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Дата планируемой госпитализации: &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;Рекомендации подкомиссии: (это &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;поле заполняется&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;в случае принятия решения об отказе или &lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;дообследовании&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:kern w:val="16"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt;): &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t xml:space="preserve"&gt; &lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Секретарь&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00D428A7" w:rsidRPr="004E7FB4" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="360" w:lineRule="auto"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="004E7FB4"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:eastAsia="Times New Roman CYR" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Печать (треугольная) Института&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidRDefault="00645BE3" w:rsidP="00645BE3"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ReferralToCommonCommission</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Направление на врачебную комиссию</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8" standalone="yes"?&gt;
+&lt;w:document xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" mc:Ignorable="w14 wp14"&gt;&lt;w:body&gt;&lt;w:p w:rsidR="00732B10" w:rsidRPr="00084B95" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:proofErr w:type="spellStart"/&gt;&lt;w:r w:rsidRPr="00084B95"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:lang w:val="en-US"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;DocumentName&lt;/w:t&gt;&lt;/w:r&gt;&lt;w:proofErr w:type="spellEnd"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00732B10" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRPr="00E71578" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00E71578"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Пациент (ФИО; возраст):&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRPr="00455FF3" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;w:u w:val="single"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Диагноз:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Код МКБ-10:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRPr="00BC410B" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:bookmarkStart w:id="0" w:name="_GoBack"/&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRPr="00BC410B" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r w:rsidRPr="00BC410B"&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Текст направления&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:bookmarkEnd w:id="0"/&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Лечащий врач:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Заведующий отделением:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="000F41A5" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0" w:line="288" w:lineRule="auto"/&gt;&lt;w:jc w:val="both"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;w:r&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman"/&gt;&lt;w:sz w:val="24"/&gt;&lt;w:szCs w:val="24"/&gt;&lt;/w:rPr&gt;&lt;w:t&gt;Печать:&lt;/w:t&gt;&lt;/w:r&gt;&lt;/w:p&gt;&lt;w:p w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidRDefault="00BC410B" w:rsidP="00BC410B"&gt;&lt;w:pPr&gt;&lt;w:spacing w:after="0"/&gt;&lt;w:jc w:val="center"/&gt;&lt;w:rPr&gt;&lt;w:rFonts w:ascii="Times New Roman" w:hAnsi="Times New Roman" w:cs="Times New Roman"/&gt;&lt;w:b/&gt;&lt;w:strike/&gt;&lt;/w:rPr&gt;&lt;/w:pPr&gt;&lt;/w:p&gt;&lt;w:sectPr w:rsidR="00084B95" w:rsidRPr="00EE03E3" w:rsidSect="00C56C6C"&gt;&lt;w:pgSz w:w="11906" w:h="16838"/&gt;&lt;w:pgMar w:top="720" w:right="720" w:bottom="720" w:left="720" w:header="708" w:footer="708" w:gutter="0"/&gt;&lt;w:cols w:space="708"/&gt;&lt;w:docGrid w:linePitch="360"/&gt;&lt;/w:sectPr&gt;&lt;/w:body&gt;&lt;/w:document&gt;</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -463,13 +587,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G6"/>
+  <x:dimension ref="A1:F16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -488,113 +612,275 @@
       <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>9</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s"/>
       <x:c r="E2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F2" s="1" t="s">
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>19</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s"/>
       <x:c r="E4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F4" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="A5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s"/>
       <x:c r="E5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F5" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:7">
-      <x:c r="A6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s"/>
       <x:c r="E6" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F6" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>10</x:v>
+      <x:c r="C7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F7" s="1" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F8" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F9" s="1" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F10" s="1" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s"/>
+      <x:c r="E11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F11" s="1" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s"/>
+      <x:c r="E12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F12" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s"/>
+      <x:c r="E13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F13" s="1" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s"/>
+      <x:c r="E14" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F14" s="1" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s"/>
+      <x:c r="E15" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F15" s="1" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s"/>
+      <x:c r="E16" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F16" s="1" t="s">
+        <x:v>66</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>